<commit_message>
Added one string in the VO classs
</commit_message>
<xml_diff>
--- a/INOW Automation Data Sheet.xlsx
+++ b/INOW Automation Data Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\InsuranceNowAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD7E3BF-495B-4E79-A774-97603FF7E318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8279C828-21CC-4DAC-A27D-D80D40A8B91D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="9" activeTab="13" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4639" uniqueCount="1589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4642" uniqueCount="1590">
   <si>
     <t>NewBussines</t>
   </si>
@@ -4819,6 +4819,9 @@
   </si>
   <si>
     <t xml:space="preserve">newBusinessVehicle2Ignore </t>
+  </si>
+  <si>
+    <t>newBusinessHastheinsuredoperatedanuninsuredmotorvehicleformorethan30daysinthepast12months</t>
   </si>
 </sst>
 </file>
@@ -9538,10 +9541,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA4E5AA-688C-484A-99F1-9AC8F41EC26C}">
-  <dimension ref="A1:D370"/>
+  <dimension ref="A1:D371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A351" workbookViewId="0">
-      <selection activeCell="C358" sqref="C358"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9668,37 +9671,37 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>1589</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>411</v>
+      <c r="C12" s="2" t="s">
+        <v>410</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>1542</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="D13" s="1"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
@@ -9706,10 +9709,10 @@
         <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1539</v>
+        <v>1542</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -9718,21 +9721,21 @@
         <v>7</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="D15" s="1"/>
+        <v>413</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>1539</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>415</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>1540</v>
-      </c>
+      <c r="C16" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="24"/>
@@ -9740,9 +9743,11 @@
         <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="D17" s="1"/>
+        <v>415</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>1540</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="24"/>
@@ -9750,29 +9755,29 @@
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>1541</v>
-      </c>
+        <v>416</v>
+      </c>
+      <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="24"/>
       <c r="B19" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="D19" s="1"/>
+      <c r="C19" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>1541</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
-      <c r="B20" s="8" t="s">
-        <v>8</v>
+      <c r="B20" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -9782,7 +9787,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -9792,7 +9797,7 @@
         <v>8</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D22" s="1"/>
     </row>
@@ -9801,8 +9806,8 @@
       <c r="B23" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>422</v>
+      <c r="C23" s="1" t="s">
+        <v>421</v>
       </c>
       <c r="D23" s="1"/>
     </row>
@@ -9812,7 +9817,7 @@
         <v>8</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D24" s="1"/>
     </row>
@@ -9822,7 +9827,7 @@
         <v>8</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D25" s="1"/>
     </row>
@@ -9831,8 +9836,8 @@
       <c r="B26" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>425</v>
+      <c r="C26" s="2" t="s">
+        <v>424</v>
       </c>
       <c r="D26" s="1"/>
     </row>
@@ -9842,7 +9847,7 @@
         <v>8</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="D27" s="1"/>
     </row>
@@ -9852,7 +9857,7 @@
         <v>8</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="D28" s="1"/>
     </row>
@@ -9862,7 +9867,7 @@
         <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D29" s="1"/>
     </row>
@@ -9871,8 +9876,8 @@
       <c r="B30" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>429</v>
+      <c r="C30" s="1" t="s">
+        <v>428</v>
       </c>
       <c r="D30" s="1"/>
     </row>
@@ -9882,7 +9887,7 @@
         <v>8</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D31" s="1"/>
     </row>
@@ -9892,7 +9897,7 @@
         <v>8</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D32" s="1"/>
     </row>
@@ -9901,8 +9906,8 @@
       <c r="B33" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>432</v>
+      <c r="C33" s="2" t="s">
+        <v>431</v>
       </c>
       <c r="D33" s="1"/>
     </row>
@@ -9912,17 +9917,17 @@
         <v>8</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>763</v>
+        <v>432</v>
       </c>
       <c r="D34" s="1"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="24"/>
-      <c r="B35" s="7" t="s">
-        <v>4</v>
+      <c r="B35" s="8" t="s">
+        <v>8</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>433</v>
+        <v>763</v>
       </c>
       <c r="D35" s="1"/>
     </row>
@@ -9931,23 +9936,21 @@
       <c r="B36" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>742</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>1546</v>
-      </c>
+      <c r="C36" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="D36" s="1"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="24"/>
       <c r="B37" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>743</v>
+      <c r="C37" s="2" t="s">
+        <v>742</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -9956,10 +9959,10 @@
         <v>4</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>744</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>1536</v>
+        <v>743</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>1547</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -9968,10 +9971,10 @@
         <v>4</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="D39" s="17" t="s">
-        <v>1545</v>
+        <v>744</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>1536</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -9980,9 +9983,11 @@
         <v>4</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>746</v>
-      </c>
-      <c r="D40" s="1"/>
+        <v>745</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>1545</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="24"/>
@@ -9990,17 +9995,17 @@
         <v>4</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="D41" s="1"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="24"/>
-      <c r="B42" s="8" t="s">
-        <v>9</v>
+      <c r="B42" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>434</v>
+        <v>747</v>
       </c>
       <c r="D42" s="1"/>
     </row>
@@ -10010,7 +10015,7 @@
         <v>9</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="D43" s="1"/>
     </row>
@@ -10020,11 +10025,9 @@
         <v>9</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="D44" s="18" t="s">
-        <v>1548</v>
-      </c>
+        <v>435</v>
+      </c>
+      <c r="D44" s="1"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="24"/>
@@ -10032,9 +10035,11 @@
         <v>9</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="D45" s="1"/>
+        <v>436</v>
+      </c>
+      <c r="D45" s="18" t="s">
+        <v>1548</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="24"/>
@@ -10042,11 +10047,9 @@
         <v>9</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>1543</v>
-      </c>
+        <v>437</v>
+      </c>
+      <c r="D46" s="1"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="24"/>
@@ -10054,10 +10057,10 @@
         <v>9</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -10066,44 +10069,44 @@
         <v>9</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="D48" s="1"/>
+        <v>439</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>1544</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="25"/>
+      <c r="A49" s="24"/>
       <c r="B49" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="D49" s="1"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="25"/>
+      <c r="B50" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="20" t="s">
+      <c r="D50" s="1"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>442</v>
-      </c>
-      <c r="D50" s="17" t="s">
-        <v>1549</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="21"/>
       <c r="B51" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -10112,10 +10115,10 @@
         <v>10</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>1553</v>
+        <v>443</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -10124,10 +10127,10 @@
         <v>10</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>445</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>1552</v>
+        <v>1553</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>1551</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -10136,7 +10139,7 @@
         <v>10</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>1554</v>
+        <v>445</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>1552</v>
@@ -10148,7 +10151,7 @@
         <v>10</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>447</v>
+        <v>1554</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>1552</v>
@@ -10160,10 +10163,10 @@
         <v>10</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>25</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -10172,9 +10175,11 @@
         <v>10</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="D57" s="1"/>
+        <v>448</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="21"/>
@@ -10182,43 +10187,43 @@
         <v>10</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="D58" s="1"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="22"/>
+      <c r="A59" s="21"/>
       <c r="B59" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="D59" s="1"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="22"/>
+      <c r="B60" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="20" t="s">
+      <c r="D60" s="1"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B60" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>452</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>1556</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="21"/>
       <c r="B61" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="D61" s="1"/>
+        <v>452</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>1556</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="21"/>
@@ -10226,11 +10231,9 @@
         <v>11</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>1576</v>
-      </c>
+        <v>453</v>
+      </c>
+      <c r="D62" s="1"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="21"/>
@@ -10238,10 +10241,10 @@
         <v>11</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>1555</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -10250,10 +10253,10 @@
         <v>11</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -10262,10 +10265,10 @@
         <v>11</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>1563</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>1562</v>
+        <v>456</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>1557</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -10274,10 +10277,10 @@
         <v>11</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>1558</v>
+        <v>1563</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>1562</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -10286,10 +10289,10 @@
         <v>11</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -10298,9 +10301,11 @@
         <v>11</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="D68" s="17"/>
+        <v>459</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>1559</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="21"/>
@@ -10308,11 +10313,9 @@
         <v>11</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1565</v>
-      </c>
-      <c r="D69" s="17" t="s">
-        <v>1564</v>
-      </c>
+        <v>460</v>
+      </c>
+      <c r="D69" s="17"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="21"/>
@@ -10320,9 +10323,11 @@
         <v>11</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="D70" s="1"/>
+        <v>1565</v>
+      </c>
+      <c r="D70" s="17" t="s">
+        <v>1564</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="21"/>
@@ -10330,11 +10335,9 @@
         <v>11</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="D71" s="17" t="s">
-        <v>1560</v>
-      </c>
+        <v>462</v>
+      </c>
+      <c r="D71" s="1"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="21"/>
@@ -10342,10 +10345,10 @@
         <v>11</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>464</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>1561</v>
+        <v>463</v>
+      </c>
+      <c r="D72" s="17" t="s">
+        <v>1560</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -10354,10 +10357,10 @@
         <v>11</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>25</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -10366,9 +10369,11 @@
         <v>11</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="D74" s="1"/>
+        <v>465</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="21"/>
@@ -10376,21 +10381,19 @@
         <v>11</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="D75" s="1"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="21"/>
       <c r="B76" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>1566</v>
-      </c>
+        <v>467</v>
+      </c>
+      <c r="D76" s="1"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="21"/>
@@ -10398,9 +10401,11 @@
         <v>12</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="D77" s="1"/>
+        <v>468</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>1566</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="21"/>
@@ -10408,17 +10413,17 @@
         <v>12</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D78" s="1"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="21"/>
       <c r="B79" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="D79" s="1"/>
     </row>
@@ -10428,7 +10433,7 @@
         <v>13</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="D80" s="1"/>
     </row>
@@ -10438,7 +10443,7 @@
         <v>13</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="D81" s="1"/>
     </row>
@@ -10448,7 +10453,7 @@
         <v>13</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D82" s="1"/>
     </row>
@@ -10458,7 +10463,7 @@
         <v>13</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D83" s="1"/>
     </row>
@@ -10468,7 +10473,7 @@
         <v>13</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D84" s="1"/>
     </row>
@@ -10478,17 +10483,17 @@
         <v>13</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D85" s="1"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="21"/>
       <c r="B86" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D86" s="1"/>
     </row>
@@ -10498,7 +10503,7 @@
         <v>14</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D87" s="1"/>
     </row>
@@ -10508,7 +10513,7 @@
         <v>14</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D88" s="1"/>
     </row>
@@ -10518,7 +10523,7 @@
         <v>14</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D89" s="1"/>
     </row>
@@ -10528,7 +10533,7 @@
         <v>14</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D90" s="1"/>
     </row>
@@ -10538,24 +10543,24 @@
         <v>14</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D91" s="1"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="21"/>
-      <c r="B92" s="7"/>
-      <c r="C92" s="1"/>
+      <c r="B92" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>483</v>
+      </c>
       <c r="D92" s="1"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="21"/>
-      <c r="B93" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>484</v>
-      </c>
+      <c r="B93" s="7"/>
+      <c r="C93" s="1"/>
       <c r="D93" s="1"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -10564,7 +10569,7 @@
         <v>11</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D94" s="1"/>
     </row>
@@ -10574,7 +10579,7 @@
         <v>11</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D95" s="1"/>
     </row>
@@ -10584,7 +10589,7 @@
         <v>11</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D96" s="1"/>
     </row>
@@ -10594,7 +10599,7 @@
         <v>11</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D97" s="1"/>
     </row>
@@ -10604,7 +10609,7 @@
         <v>11</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D98" s="1"/>
     </row>
@@ -10614,7 +10619,7 @@
         <v>11</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D99" s="1"/>
     </row>
@@ -10624,7 +10629,7 @@
         <v>11</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D100" s="1"/>
     </row>
@@ -10634,7 +10639,7 @@
         <v>11</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D101" s="1"/>
     </row>
@@ -10644,7 +10649,7 @@
         <v>11</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D102" s="1"/>
     </row>
@@ -10654,7 +10659,7 @@
         <v>11</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D103" s="1"/>
     </row>
@@ -10664,7 +10669,7 @@
         <v>11</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D104" s="1"/>
     </row>
@@ -10674,7 +10679,7 @@
         <v>11</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>804</v>
+        <v>495</v>
       </c>
       <c r="D105" s="1"/>
     </row>
@@ -10684,7 +10689,7 @@
         <v>11</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>496</v>
+        <v>804</v>
       </c>
       <c r="D106" s="1"/>
     </row>
@@ -10694,7 +10699,7 @@
         <v>11</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D107" s="1"/>
     </row>
@@ -10704,17 +10709,17 @@
         <v>11</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="D108" s="1"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="21"/>
       <c r="B109" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D109" s="1"/>
     </row>
@@ -10724,7 +10729,7 @@
         <v>12</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D110" s="1"/>
     </row>
@@ -10734,17 +10739,17 @@
         <v>12</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="D111" s="1"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="21"/>
       <c r="B112" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="D112" s="1"/>
     </row>
@@ -10754,7 +10759,7 @@
         <v>13</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D113" s="1"/>
     </row>
@@ -10764,7 +10769,7 @@
         <v>13</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D114" s="1"/>
     </row>
@@ -10774,7 +10779,7 @@
         <v>13</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D115" s="1"/>
     </row>
@@ -10784,7 +10789,7 @@
         <v>13</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D116" s="1"/>
     </row>
@@ -10794,7 +10799,7 @@
         <v>13</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="D117" s="1"/>
     </row>
@@ -10804,17 +10809,17 @@
         <v>13</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D118" s="1"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="21"/>
       <c r="B119" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D119" s="1"/>
     </row>
@@ -10824,7 +10829,7 @@
         <v>14</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D120" s="1"/>
     </row>
@@ -10834,7 +10839,7 @@
         <v>14</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D121" s="1"/>
     </row>
@@ -10844,7 +10849,7 @@
         <v>14</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D122" s="1"/>
     </row>
@@ -10854,7 +10859,7 @@
         <v>14</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D123" s="1"/>
     </row>
@@ -10864,24 +10869,24 @@
         <v>14</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D124" s="1"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="21"/>
-      <c r="B125" s="7"/>
-      <c r="C125" s="1"/>
+      <c r="B125" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>514</v>
+      </c>
       <c r="D125" s="1"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="21"/>
-      <c r="B126" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C126" s="1" t="s">
-        <v>515</v>
-      </c>
+      <c r="B126" s="7"/>
+      <c r="C126" s="1"/>
       <c r="D126" s="1"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -10890,7 +10895,7 @@
         <v>11</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D127" s="1"/>
     </row>
@@ -10900,7 +10905,7 @@
         <v>11</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D128" s="1"/>
     </row>
@@ -10910,7 +10915,7 @@
         <v>11</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="D129" s="1"/>
     </row>
@@ -10920,7 +10925,7 @@
         <v>11</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D130" s="1"/>
     </row>
@@ -10930,7 +10935,7 @@
         <v>11</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D131" s="1"/>
     </row>
@@ -10940,7 +10945,7 @@
         <v>11</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D132" s="1"/>
     </row>
@@ -10950,7 +10955,7 @@
         <v>11</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="D133" s="1"/>
     </row>
@@ -10960,7 +10965,7 @@
         <v>11</v>
       </c>
       <c r="C134" s="1" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D134" s="1"/>
     </row>
@@ -10970,7 +10975,7 @@
         <v>11</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D135" s="1"/>
     </row>
@@ -10980,7 +10985,7 @@
         <v>11</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="D136" s="1"/>
     </row>
@@ -10990,7 +10995,7 @@
         <v>11</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D137" s="1"/>
     </row>
@@ -11000,7 +11005,7 @@
         <v>11</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>805</v>
+        <v>526</v>
       </c>
       <c r="D138" s="1"/>
     </row>
@@ -11010,7 +11015,7 @@
         <v>11</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>527</v>
+        <v>805</v>
       </c>
       <c r="D139" s="1"/>
     </row>
@@ -11020,7 +11025,7 @@
         <v>11</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D140" s="1"/>
     </row>
@@ -11030,17 +11035,17 @@
         <v>11</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D141" s="1"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="21"/>
       <c r="B142" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C142" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D142" s="1"/>
     </row>
@@ -11050,7 +11055,7 @@
         <v>12</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D143" s="1"/>
     </row>
@@ -11060,17 +11065,17 @@
         <v>12</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D144" s="1"/>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="21"/>
       <c r="B145" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D145" s="1"/>
     </row>
@@ -11080,7 +11085,7 @@
         <v>13</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D146" s="1"/>
     </row>
@@ -11090,7 +11095,7 @@
         <v>13</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="D147" s="1"/>
     </row>
@@ -11100,7 +11105,7 @@
         <v>13</v>
       </c>
       <c r="C148" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="D148" s="1"/>
     </row>
@@ -11110,7 +11115,7 @@
         <v>13</v>
       </c>
       <c r="C149" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="D149" s="1"/>
     </row>
@@ -11120,7 +11125,7 @@
         <v>13</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="D150" s="1"/>
     </row>
@@ -11130,17 +11135,17 @@
         <v>13</v>
       </c>
       <c r="C151" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D151" s="1"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="21"/>
       <c r="B152" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C152" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="D152" s="1"/>
     </row>
@@ -11150,7 +11155,7 @@
         <v>14</v>
       </c>
       <c r="C153" s="1" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D153" s="1"/>
     </row>
@@ -11160,7 +11165,7 @@
         <v>14</v>
       </c>
       <c r="C154" s="1" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="D154" s="1"/>
     </row>
@@ -11170,7 +11175,7 @@
         <v>14</v>
       </c>
       <c r="C155" s="1" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D155" s="1"/>
     </row>
@@ -11180,39 +11185,39 @@
         <v>14</v>
       </c>
       <c r="C156" s="1" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D156" s="1"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="22"/>
+      <c r="A157" s="21"/>
       <c r="B157" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C157" s="1" t="s">
+        <v>544</v>
+      </c>
+      <c r="D157" s="1"/>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="22"/>
+      <c r="B158" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C158" s="1" t="s">
         <v>545</v>
       </c>
-      <c r="D157" s="1"/>
-    </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="20" t="s">
+      <c r="D158" s="1"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B158" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>546</v>
-      </c>
-      <c r="D158" s="1"/>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="21"/>
       <c r="B159" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D159" s="1"/>
     </row>
@@ -11222,7 +11227,7 @@
         <v>15</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D160" s="1"/>
     </row>
@@ -11232,7 +11237,7 @@
         <v>15</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="D161" s="1"/>
     </row>
@@ -11242,7 +11247,7 @@
         <v>15</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="D162" s="1"/>
     </row>
@@ -11252,7 +11257,7 @@
         <v>15</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D163" s="1"/>
     </row>
@@ -11262,7 +11267,7 @@
         <v>15</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D164" s="1"/>
     </row>
@@ -11272,7 +11277,7 @@
         <v>15</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="D165" s="1"/>
     </row>
@@ -11282,27 +11287,27 @@
         <v>15</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D166" s="1"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="21"/>
-      <c r="B167" s="11" t="s">
+      <c r="B167" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D167" s="1"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="21"/>
-      <c r="B168" s="7" t="s">
+      <c r="B168" s="11" t="s">
         <v>15</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D168" s="1"/>
     </row>
@@ -11312,7 +11317,7 @@
         <v>15</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D169" s="1"/>
     </row>
@@ -11322,7 +11327,7 @@
         <v>15</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D170" s="1"/>
     </row>
@@ -11332,7 +11337,7 @@
         <v>15</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D171" s="1"/>
     </row>
@@ -11342,43 +11347,43 @@
         <v>15</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D172" s="1"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="22"/>
+      <c r="A173" s="21"/>
       <c r="B173" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C173" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="D173" s="1"/>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" s="22"/>
+      <c r="B174" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C174" s="1" t="s">
         <v>561</v>
       </c>
-      <c r="D173" s="1"/>
-    </row>
-    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="20" t="s">
+      <c r="D174" s="1"/>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B174" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C174" s="1" t="s">
+      <c r="B175" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C175" s="1" t="s">
         <v>562</v>
       </c>
-      <c r="D174" s="17" t="s">
+      <c r="D175" s="17" t="s">
         <v>1567</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="21"/>
-      <c r="B175" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C175" s="1" t="s">
-        <v>563</v>
-      </c>
-      <c r="D175" s="1"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="21"/>
@@ -11386,7 +11391,7 @@
         <v>16</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D176" s="1"/>
     </row>
@@ -11396,7 +11401,7 @@
         <v>16</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D177" s="1"/>
     </row>
@@ -11406,7 +11411,7 @@
         <v>16</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D178" s="1"/>
     </row>
@@ -11416,7 +11421,7 @@
         <v>16</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D179" s="1"/>
     </row>
@@ -11425,8 +11430,8 @@
       <c r="B180" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C180" s="12" t="s">
-        <v>568</v>
+      <c r="C180" s="1" t="s">
+        <v>567</v>
       </c>
       <c r="D180" s="1"/>
     </row>
@@ -11435,8 +11440,8 @@
       <c r="B181" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C181" s="1" t="s">
-        <v>569</v>
+      <c r="C181" s="12" t="s">
+        <v>568</v>
       </c>
       <c r="D181" s="1"/>
     </row>
@@ -11446,7 +11451,7 @@
         <v>16</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D182" s="1"/>
     </row>
@@ -11456,7 +11461,7 @@
         <v>16</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D183" s="1"/>
     </row>
@@ -11466,11 +11471,9 @@
         <v>16</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="D184" s="1" t="s">
-        <v>1568</v>
-      </c>
+        <v>571</v>
+      </c>
+      <c r="D184" s="1"/>
     </row>
     <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="21"/>
@@ -11478,10 +11481,10 @@
         <v>16</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>1572</v>
+        <v>572</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
@@ -11490,9 +11493,11 @@
         <v>16</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>574</v>
-      </c>
-      <c r="D186" s="1"/>
+        <v>1572</v>
+      </c>
+      <c r="D186" s="1" t="s">
+        <v>1569</v>
+      </c>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="21"/>
@@ -11500,7 +11505,7 @@
         <v>16</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D187" s="1"/>
     </row>
@@ -11510,7 +11515,7 @@
         <v>16</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D188" s="1"/>
     </row>
@@ -11520,7 +11525,7 @@
         <v>16</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D189" s="1"/>
     </row>
@@ -11530,7 +11535,7 @@
         <v>16</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D190" s="1"/>
     </row>
@@ -11540,11 +11545,9 @@
         <v>16</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>579</v>
-      </c>
-      <c r="D191" s="1" t="s">
-        <v>1570</v>
-      </c>
+        <v>578</v>
+      </c>
+      <c r="D191" s="1"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="21"/>
@@ -11552,7 +11555,7 @@
         <v>16</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>1570</v>
@@ -11564,10 +11567,10 @@
         <v>16</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
@@ -11576,7 +11579,7 @@
         <v>16</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>1573</v>
+        <v>581</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>1571</v>
@@ -11588,7 +11591,7 @@
         <v>16</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>1571</v>
@@ -11600,9 +11603,11 @@
         <v>16</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>584</v>
-      </c>
-      <c r="D196" s="1"/>
+        <v>1574</v>
+      </c>
+      <c r="D196" s="1" t="s">
+        <v>1571</v>
+      </c>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="21"/>
@@ -11610,7 +11615,7 @@
         <v>16</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D197" s="1"/>
     </row>
@@ -11620,7 +11625,7 @@
         <v>16</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D198" s="1"/>
     </row>
@@ -11630,7 +11635,7 @@
         <v>16</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D199" s="1"/>
     </row>
@@ -11640,7 +11645,7 @@
         <v>16</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D200" s="1"/>
     </row>
@@ -11650,7 +11655,7 @@
         <v>16</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D201" s="1"/>
     </row>
@@ -11660,7 +11665,7 @@
         <v>16</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D202" s="1"/>
     </row>
@@ -11670,24 +11675,24 @@
         <v>16</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="D203" s="1"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="21"/>
-      <c r="B204" s="10"/>
-      <c r="C204" s="1"/>
+      <c r="B204" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C204" s="1" t="s">
+        <v>591</v>
+      </c>
       <c r="D204" s="1"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="21"/>
-      <c r="B205" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C205" s="1" t="s">
-        <v>592</v>
-      </c>
+      <c r="B205" s="10"/>
+      <c r="C205" s="1"/>
       <c r="D205" s="1"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
@@ -11696,7 +11701,7 @@
         <v>16</v>
       </c>
       <c r="C206" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D206" s="1"/>
     </row>
@@ -11706,7 +11711,7 @@
         <v>16</v>
       </c>
       <c r="C207" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D207" s="1"/>
     </row>
@@ -11716,7 +11721,7 @@
         <v>16</v>
       </c>
       <c r="C208" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D208" s="1"/>
     </row>
@@ -11726,7 +11731,7 @@
         <v>16</v>
       </c>
       <c r="C209" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D209" s="1"/>
     </row>
@@ -11736,7 +11741,7 @@
         <v>16</v>
       </c>
       <c r="C210" s="1" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D210" s="1"/>
     </row>
@@ -11745,8 +11750,8 @@
       <c r="B211" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C211" s="12" t="s">
-        <v>598</v>
+      <c r="C211" s="1" t="s">
+        <v>597</v>
       </c>
       <c r="D211" s="1"/>
     </row>
@@ -11755,8 +11760,8 @@
       <c r="B212" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C212" s="1" t="s">
-        <v>599</v>
+      <c r="C212" s="12" t="s">
+        <v>598</v>
       </c>
       <c r="D212" s="1"/>
     </row>
@@ -11766,7 +11771,7 @@
         <v>16</v>
       </c>
       <c r="C213" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D213" s="1"/>
     </row>
@@ -11776,7 +11781,7 @@
         <v>16</v>
       </c>
       <c r="C214" s="1" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D214" s="1"/>
     </row>
@@ -11786,7 +11791,7 @@
         <v>16</v>
       </c>
       <c r="C215" s="1" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D215" s="1"/>
     </row>
@@ -11796,7 +11801,7 @@
         <v>16</v>
       </c>
       <c r="C216" s="1" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="D216" s="1"/>
     </row>
@@ -11806,7 +11811,7 @@
         <v>16</v>
       </c>
       <c r="C217" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="D217" s="1"/>
     </row>
@@ -11816,7 +11821,7 @@
         <v>16</v>
       </c>
       <c r="C218" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D218" s="1"/>
     </row>
@@ -11826,7 +11831,7 @@
         <v>16</v>
       </c>
       <c r="C219" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="D219" s="1"/>
     </row>
@@ -11836,7 +11841,7 @@
         <v>16</v>
       </c>
       <c r="C220" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D220" s="1"/>
     </row>
@@ -11846,7 +11851,7 @@
         <v>16</v>
       </c>
       <c r="C221" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D221" s="1"/>
     </row>
@@ -11856,7 +11861,7 @@
         <v>16</v>
       </c>
       <c r="C222" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D222" s="1"/>
     </row>
@@ -11866,7 +11871,7 @@
         <v>16</v>
       </c>
       <c r="C223" s="1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D223" s="1"/>
     </row>
@@ -11876,7 +11881,7 @@
         <v>16</v>
       </c>
       <c r="C224" s="1" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D224" s="1"/>
     </row>
@@ -11886,7 +11891,7 @@
         <v>16</v>
       </c>
       <c r="C225" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D225" s="1"/>
     </row>
@@ -11896,7 +11901,7 @@
         <v>16</v>
       </c>
       <c r="C226" s="1" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="D226" s="1"/>
     </row>
@@ -11906,7 +11911,7 @@
         <v>16</v>
       </c>
       <c r="C227" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D227" s="1"/>
     </row>
@@ -11916,7 +11921,7 @@
         <v>16</v>
       </c>
       <c r="C228" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D228" s="1"/>
     </row>
@@ -11926,7 +11931,7 @@
         <v>16</v>
       </c>
       <c r="C229" s="1" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D229" s="1"/>
     </row>
@@ -11936,7 +11941,7 @@
         <v>16</v>
       </c>
       <c r="C230" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D230" s="1"/>
     </row>
@@ -11946,7 +11951,7 @@
         <v>16</v>
       </c>
       <c r="C231" s="1" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D231" s="1"/>
     </row>
@@ -11956,7 +11961,7 @@
         <v>16</v>
       </c>
       <c r="C232" s="1" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D232" s="1"/>
     </row>
@@ -11966,7 +11971,7 @@
         <v>16</v>
       </c>
       <c r="C233" s="1" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D233" s="1"/>
     </row>
@@ -11976,24 +11981,24 @@
         <v>16</v>
       </c>
       <c r="C234" s="1" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D234" s="1"/>
     </row>
     <row r="235" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A235" s="21"/>
-      <c r="B235" s="7"/>
-      <c r="C235" s="1"/>
+      <c r="B235" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C235" s="1" t="s">
+        <v>621</v>
+      </c>
       <c r="D235" s="1"/>
     </row>
     <row r="236" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A236" s="21"/>
-      <c r="B236" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>622</v>
-      </c>
+      <c r="B236" s="7"/>
+      <c r="C236" s="1"/>
       <c r="D236" s="1"/>
     </row>
     <row r="237" spans="1:4" x14ac:dyDescent="0.25">
@@ -12002,7 +12007,7 @@
         <v>16</v>
       </c>
       <c r="C237" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D237" s="1"/>
     </row>
@@ -12012,7 +12017,7 @@
         <v>16</v>
       </c>
       <c r="C238" s="1" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D238" s="1"/>
     </row>
@@ -12022,7 +12027,7 @@
         <v>16</v>
       </c>
       <c r="C239" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D239" s="1"/>
     </row>
@@ -12032,7 +12037,7 @@
         <v>16</v>
       </c>
       <c r="C240" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D240" s="1"/>
     </row>
@@ -12042,7 +12047,7 @@
         <v>16</v>
       </c>
       <c r="C241" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D241" s="1"/>
     </row>
@@ -12051,8 +12056,8 @@
       <c r="B242" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C242" s="12" t="s">
-        <v>628</v>
+      <c r="C242" s="1" t="s">
+        <v>627</v>
       </c>
       <c r="D242" s="1"/>
     </row>
@@ -12061,8 +12066,8 @@
       <c r="B243" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C243" s="1" t="s">
-        <v>629</v>
+      <c r="C243" s="12" t="s">
+        <v>628</v>
       </c>
       <c r="D243" s="1"/>
     </row>
@@ -12072,7 +12077,7 @@
         <v>16</v>
       </c>
       <c r="C244" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D244" s="1"/>
     </row>
@@ -12082,7 +12087,7 @@
         <v>16</v>
       </c>
       <c r="C245" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D245" s="1"/>
     </row>
@@ -12092,7 +12097,7 @@
         <v>16</v>
       </c>
       <c r="C246" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D246" s="1"/>
     </row>
@@ -12102,7 +12107,7 @@
         <v>16</v>
       </c>
       <c r="C247" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="D247" s="1"/>
     </row>
@@ -12112,7 +12117,7 @@
         <v>16</v>
       </c>
       <c r="C248" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D248" s="1"/>
     </row>
@@ -12122,7 +12127,7 @@
         <v>16</v>
       </c>
       <c r="C249" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D249" s="1"/>
     </row>
@@ -12132,7 +12137,7 @@
         <v>16</v>
       </c>
       <c r="C250" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D250" s="1"/>
     </row>
@@ -12142,7 +12147,7 @@
         <v>16</v>
       </c>
       <c r="C251" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D251" s="1"/>
     </row>
@@ -12152,7 +12157,7 @@
         <v>16</v>
       </c>
       <c r="C252" s="1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="D252" s="1"/>
     </row>
@@ -12162,7 +12167,7 @@
         <v>16</v>
       </c>
       <c r="C253" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D253" s="1"/>
     </row>
@@ -12172,7 +12177,7 @@
         <v>16</v>
       </c>
       <c r="C254" s="1" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D254" s="1"/>
     </row>
@@ -12182,7 +12187,7 @@
         <v>16</v>
       </c>
       <c r="C255" s="1" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D255" s="1"/>
     </row>
@@ -12192,7 +12197,7 @@
         <v>16</v>
       </c>
       <c r="C256" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D256" s="1"/>
     </row>
@@ -12202,7 +12207,7 @@
         <v>16</v>
       </c>
       <c r="C257" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D257" s="1"/>
     </row>
@@ -12212,7 +12217,7 @@
         <v>16</v>
       </c>
       <c r="C258" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D258" s="1"/>
     </row>
@@ -12222,7 +12227,7 @@
         <v>16</v>
       </c>
       <c r="C259" s="1" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D259" s="1"/>
     </row>
@@ -12232,7 +12237,7 @@
         <v>16</v>
       </c>
       <c r="C260" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D260" s="1"/>
     </row>
@@ -12242,7 +12247,7 @@
         <v>16</v>
       </c>
       <c r="C261" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D261" s="1"/>
     </row>
@@ -12252,7 +12257,7 @@
         <v>16</v>
       </c>
       <c r="C262" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D262" s="1"/>
     </row>
@@ -12262,7 +12267,7 @@
         <v>16</v>
       </c>
       <c r="C263" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="D263" s="1"/>
     </row>
@@ -12272,7 +12277,7 @@
         <v>16</v>
       </c>
       <c r="C264" s="1" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="D264" s="1"/>
     </row>
@@ -12282,17 +12287,17 @@
         <v>16</v>
       </c>
       <c r="C265" s="1" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="D265" s="1"/>
     </row>
     <row r="266" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A266" s="21"/>
-      <c r="B266" s="10" t="s">
-        <v>17</v>
+      <c r="B266" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="C266" s="1" t="s">
-        <v>751</v>
+        <v>651</v>
       </c>
       <c r="D266" s="1"/>
     </row>
@@ -12302,7 +12307,7 @@
         <v>17</v>
       </c>
       <c r="C267" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D267" s="1"/>
     </row>
@@ -12312,7 +12317,7 @@
         <v>17</v>
       </c>
       <c r="C268" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="D268" s="1"/>
     </row>
@@ -12322,7 +12327,7 @@
         <v>17</v>
       </c>
       <c r="C269" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="D269" s="1"/>
     </row>
@@ -12332,7 +12337,7 @@
         <v>17</v>
       </c>
       <c r="C270" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="D270" s="1"/>
     </row>
@@ -12342,7 +12347,7 @@
         <v>17</v>
       </c>
       <c r="C271" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D271" s="1"/>
     </row>
@@ -12352,7 +12357,7 @@
         <v>17</v>
       </c>
       <c r="C272" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="D272" s="1"/>
     </row>
@@ -12362,7 +12367,7 @@
         <v>17</v>
       </c>
       <c r="C273" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="D273" s="1"/>
     </row>
@@ -12372,7 +12377,7 @@
         <v>17</v>
       </c>
       <c r="C274" s="1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="D274" s="1"/>
     </row>
@@ -12382,7 +12387,7 @@
         <v>17</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="D275" s="1"/>
     </row>
@@ -12392,39 +12397,39 @@
         <v>17</v>
       </c>
       <c r="C276" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="D276" s="1"/>
     </row>
     <row r="277" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A277" s="22"/>
+      <c r="A277" s="21"/>
       <c r="B277" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C277" s="12" t="s">
+      <c r="C277" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="D277" s="1"/>
+    </row>
+    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A278" s="22"/>
+      <c r="B278" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C278" s="12" t="s">
         <v>762</v>
       </c>
-      <c r="D277" s="1"/>
-    </row>
-    <row r="278" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A278" s="20" t="s">
+      <c r="D278" s="1"/>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A279" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B278" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C278" s="1" t="s">
+      <c r="B279" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C279" s="1" t="s">
         <v>652</v>
-      </c>
-      <c r="D278" s="1"/>
-    </row>
-    <row r="279" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A279" s="21"/>
-      <c r="B279" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C279" s="1" t="s">
-        <v>653</v>
       </c>
       <c r="D279" s="1"/>
     </row>
@@ -12434,7 +12439,7 @@
         <v>18</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="D280" s="1"/>
     </row>
@@ -12444,7 +12449,7 @@
         <v>18</v>
       </c>
       <c r="C281" s="1" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="D281" s="1"/>
     </row>
@@ -12454,7 +12459,7 @@
         <v>18</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D282" s="1"/>
     </row>
@@ -12464,7 +12469,7 @@
         <v>18</v>
       </c>
       <c r="C283" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="D283" s="1"/>
     </row>
@@ -12474,7 +12479,7 @@
         <v>18</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D284" s="1"/>
     </row>
@@ -12484,7 +12489,7 @@
         <v>18</v>
       </c>
       <c r="C285" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D285" s="1"/>
     </row>
@@ -12494,7 +12499,7 @@
         <v>18</v>
       </c>
       <c r="C286" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D286" s="1"/>
     </row>
@@ -12504,7 +12509,7 @@
         <v>18</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D287" s="1"/>
     </row>
@@ -12514,7 +12519,7 @@
         <v>18</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="D288" s="1"/>
     </row>
@@ -12524,7 +12529,7 @@
         <v>18</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D289" s="1"/>
     </row>
@@ -12534,7 +12539,7 @@
         <v>18</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>748</v>
+        <v>663</v>
       </c>
       <c r="D290" s="1"/>
     </row>
@@ -12544,7 +12549,7 @@
         <v>18</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>664</v>
+        <v>748</v>
       </c>
       <c r="D291" s="1"/>
     </row>
@@ -12554,7 +12559,7 @@
         <v>18</v>
       </c>
       <c r="C292" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="D292" s="1"/>
     </row>
@@ -12564,7 +12569,7 @@
         <v>18</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="D293" s="1"/>
     </row>
@@ -12574,7 +12579,7 @@
         <v>18</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="D294" s="1"/>
     </row>
@@ -12584,7 +12589,7 @@
         <v>18</v>
       </c>
       <c r="C295" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="D295" s="1"/>
     </row>
@@ -12594,7 +12599,7 @@
         <v>18</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="D296" s="1"/>
     </row>
@@ -12604,7 +12609,7 @@
         <v>18</v>
       </c>
       <c r="C297" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="D297" s="1"/>
     </row>
@@ -12614,7 +12619,7 @@
         <v>18</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D298" s="1"/>
     </row>
@@ -12624,7 +12629,7 @@
         <v>18</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="D299" s="1"/>
     </row>
@@ -12634,7 +12639,7 @@
         <v>18</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D300" s="1"/>
     </row>
@@ -12644,7 +12649,7 @@
         <v>18</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D301" s="1"/>
     </row>
@@ -12654,7 +12659,7 @@
         <v>18</v>
       </c>
       <c r="C302" s="1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="D302" s="1"/>
     </row>
@@ -12664,7 +12669,7 @@
         <v>18</v>
       </c>
       <c r="C303" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="D303" s="1"/>
     </row>
@@ -12674,7 +12679,7 @@
         <v>18</v>
       </c>
       <c r="C304" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D304" s="1"/>
     </row>
@@ -12684,7 +12689,7 @@
         <v>18</v>
       </c>
       <c r="C305" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D305" s="1"/>
     </row>
@@ -12694,7 +12699,7 @@
         <v>18</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D306" s="1"/>
     </row>
@@ -12704,7 +12709,7 @@
         <v>18</v>
       </c>
       <c r="C307" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D307" s="1"/>
     </row>
@@ -12714,7 +12719,7 @@
         <v>18</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>749</v>
+        <v>680</v>
       </c>
       <c r="D308" s="1"/>
     </row>
@@ -12724,7 +12729,7 @@
         <v>18</v>
       </c>
       <c r="C309" s="1" t="s">
-        <v>681</v>
+        <v>749</v>
       </c>
       <c r="D309" s="1"/>
     </row>
@@ -12734,7 +12739,7 @@
         <v>18</v>
       </c>
       <c r="C310" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D310" s="1"/>
     </row>
@@ -12744,7 +12749,7 @@
         <v>18</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D311" s="1"/>
     </row>
@@ -12754,7 +12759,7 @@
         <v>18</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D312" s="1"/>
     </row>
@@ -12764,7 +12769,7 @@
         <v>18</v>
       </c>
       <c r="C313" s="1" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D313" s="1"/>
     </row>
@@ -12774,7 +12779,7 @@
         <v>18</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D314" s="1"/>
     </row>
@@ -12784,7 +12789,7 @@
         <v>18</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D315" s="1"/>
     </row>
@@ -12794,7 +12799,7 @@
         <v>18</v>
       </c>
       <c r="C316" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="D316" s="1"/>
     </row>
@@ -12804,7 +12809,7 @@
         <v>18</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D317" s="1"/>
     </row>
@@ -12814,7 +12819,7 @@
         <v>18</v>
       </c>
       <c r="C318" s="1" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D318" s="1"/>
     </row>
@@ -12824,7 +12829,7 @@
         <v>18</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D319" s="1"/>
     </row>
@@ -12834,7 +12839,7 @@
         <v>18</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="D320" s="1"/>
     </row>
@@ -12844,7 +12849,7 @@
         <v>18</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="D321" s="1"/>
     </row>
@@ -12854,7 +12859,7 @@
         <v>18</v>
       </c>
       <c r="C322" s="1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D322" s="1"/>
     </row>
@@ -12864,7 +12869,7 @@
         <v>18</v>
       </c>
       <c r="C323" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D323" s="1"/>
     </row>
@@ -12874,7 +12879,7 @@
         <v>18</v>
       </c>
       <c r="C324" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="D324" s="1"/>
     </row>
@@ -12884,7 +12889,7 @@
         <v>18</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="D325" s="1"/>
     </row>
@@ -12894,7 +12899,7 @@
         <v>18</v>
       </c>
       <c r="C326" s="1" t="s">
-        <v>750</v>
+        <v>697</v>
       </c>
       <c r="D326" s="1"/>
     </row>
@@ -12904,7 +12909,7 @@
         <v>18</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>698</v>
+        <v>750</v>
       </c>
       <c r="D327" s="1"/>
     </row>
@@ -12914,7 +12919,7 @@
         <v>18</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="D328" s="1"/>
     </row>
@@ -12923,8 +12928,8 @@
       <c r="B329" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C329" s="12" t="s">
-        <v>700</v>
+      <c r="C329" s="1" t="s">
+        <v>699</v>
       </c>
       <c r="D329" s="1"/>
     </row>
@@ -12933,40 +12938,40 @@
       <c r="B330" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C330" s="1" t="s">
+      <c r="C330" s="12" t="s">
+        <v>700</v>
+      </c>
+      <c r="D330" s="1"/>
+    </row>
+    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A331" s="21"/>
+      <c r="B331" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C331" s="1" t="s">
         <v>701</v>
       </c>
-      <c r="D330" s="1"/>
-    </row>
-    <row r="331" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A331" s="22"/>
-      <c r="B331" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C331" s="1" t="s">
+      <c r="D331" s="1"/>
+    </row>
+    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A332" s="22"/>
+      <c r="B332" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C332" s="1" t="s">
         <v>702</v>
       </c>
-      <c r="D331" s="1"/>
-    </row>
-    <row r="332" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A332" s="20" t="s">
+      <c r="D332" s="1"/>
+    </row>
+    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A333" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B332" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C332" s="1" t="s">
-        <v>703</v>
-      </c>
-      <c r="D332" s="1"/>
-    </row>
-    <row r="333" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A333" s="21"/>
       <c r="B333" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D333" s="1"/>
     </row>
@@ -12976,7 +12981,7 @@
         <v>19</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D334" s="1"/>
     </row>
@@ -12986,7 +12991,7 @@
         <v>19</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D335" s="1"/>
     </row>
@@ -12996,7 +13001,7 @@
         <v>19</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="D336" s="1"/>
     </row>
@@ -13006,7 +13011,7 @@
         <v>19</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="D337" s="1"/>
     </row>
@@ -13016,7 +13021,7 @@
         <v>19</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D338" s="1"/>
     </row>
@@ -13026,7 +13031,7 @@
         <v>19</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D339" s="1"/>
     </row>
@@ -13036,7 +13041,7 @@
         <v>19</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="D340" s="1"/>
     </row>
@@ -13046,7 +13051,7 @@
         <v>19</v>
       </c>
       <c r="C341" s="1" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="D341" s="1"/>
     </row>
@@ -13056,7 +13061,7 @@
         <v>19</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D342" s="1"/>
     </row>
@@ -13066,7 +13071,7 @@
         <v>19</v>
       </c>
       <c r="C343" s="1" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D343" s="1"/>
     </row>
@@ -13076,7 +13081,7 @@
         <v>19</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="D344" s="1"/>
     </row>
@@ -13086,7 +13091,7 @@
         <v>19</v>
       </c>
       <c r="C345" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="D345" s="1"/>
     </row>
@@ -13096,7 +13101,7 @@
         <v>19</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="D346" s="1"/>
     </row>
@@ -13106,7 +13111,7 @@
         <v>19</v>
       </c>
       <c r="C347" s="1" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="D347" s="1"/>
     </row>
@@ -13116,7 +13121,7 @@
         <v>19</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="D348" s="1"/>
     </row>
@@ -13126,7 +13131,7 @@
         <v>19</v>
       </c>
       <c r="C349" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="D349" s="1"/>
     </row>
@@ -13136,7 +13141,7 @@
         <v>19</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="D350" s="1"/>
     </row>
@@ -13146,7 +13151,7 @@
         <v>19</v>
       </c>
       <c r="C351" s="1" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="D351" s="1"/>
     </row>
@@ -13156,81 +13161,81 @@
         <v>19</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="D352" s="1"/>
     </row>
     <row r="353" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A353" s="22"/>
+      <c r="A353" s="21"/>
       <c r="B353" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C353" s="1" t="s">
+        <v>723</v>
+      </c>
+      <c r="D353" s="1"/>
+    </row>
+    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A354" s="22"/>
+      <c r="B354" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C354" s="1" t="s">
         <v>724</v>
-      </c>
-      <c r="D353" s="1"/>
-    </row>
-    <row r="354" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A354" s="1"/>
-      <c r="B354" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C354" s="1" t="s">
-        <v>725</v>
       </c>
       <c r="D354" s="1"/>
     </row>
     <row r="355" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A355" s="1"/>
-      <c r="B355" s="7"/>
+      <c r="B355" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="C355" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="D355" s="1"/>
     </row>
     <row r="356" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A356" s="1"/>
-      <c r="B356" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="B356" s="7"/>
       <c r="C356" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="D356" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>726</v>
+      </c>
+      <c r="D356" s="1"/>
     </row>
     <row r="357" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A357" s="1"/>
       <c r="B357" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C357" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="D357" s="1"/>
+        <v>727</v>
+      </c>
+      <c r="D357" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="358" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A358" s="1"/>
       <c r="B358" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C358" s="2" t="s">
-        <v>1586</v>
-      </c>
-      <c r="D358" s="1" t="s">
-        <v>1571</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="C358" s="1" t="s">
+        <v>728</v>
+      </c>
+      <c r="D358" s="1"/>
     </row>
     <row r="359" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A359" s="1"/>
       <c r="B359" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C359" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="D359" s="1"/>
+      <c r="C359" s="2" t="s">
+        <v>1586</v>
+      </c>
+      <c r="D359" s="1" t="s">
+        <v>1571</v>
+      </c>
     </row>
     <row r="360" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A360" s="1"/>
@@ -13238,7 +13243,7 @@
         <v>21</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="D360" s="1"/>
     </row>
@@ -13248,7 +13253,7 @@
         <v>21</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="D361" s="1"/>
     </row>
@@ -13258,7 +13263,7 @@
         <v>21</v>
       </c>
       <c r="C362" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="D362" s="1"/>
     </row>
@@ -13268,7 +13273,7 @@
         <v>21</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="D363" s="1"/>
     </row>
@@ -13278,7 +13283,7 @@
         <v>21</v>
       </c>
       <c r="C364" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="D364" s="1"/>
     </row>
@@ -13288,7 +13293,7 @@
         <v>21</v>
       </c>
       <c r="C365" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="D365" s="1"/>
     </row>
@@ -13298,7 +13303,7 @@
         <v>21</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="D366" s="1"/>
     </row>
@@ -13308,17 +13313,17 @@
         <v>21</v>
       </c>
       <c r="C367" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="D367" s="1"/>
     </row>
     <row r="368" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A368" s="1"/>
       <c r="B368" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C368" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="D368" s="1"/>
     </row>
@@ -13328,33 +13333,43 @@
         <v>22</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="D369" s="1"/>
     </row>
     <row r="370" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A370" s="1"/>
       <c r="B370" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C370" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="D370" s="1"/>
+    </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A371" s="1"/>
+      <c r="B371" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C370" s="1" t="s">
+      <c r="C371" s="1" t="s">
         <v>741</v>
       </c>
-      <c r="D370" s="1"/>
+      <c r="D371" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A278:A331"/>
-    <mergeCell ref="A332:A353"/>
+    <mergeCell ref="A279:A332"/>
+    <mergeCell ref="A333:A354"/>
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A49"/>
-    <mergeCell ref="A50:A59"/>
-    <mergeCell ref="A60:A157"/>
-    <mergeCell ref="A158:A173"/>
-    <mergeCell ref="A174:A277"/>
+    <mergeCell ref="A3:A50"/>
+    <mergeCell ref="A51:A60"/>
+    <mergeCell ref="A61:A158"/>
+    <mergeCell ref="A159:A174"/>
+    <mergeCell ref="A175:A278"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D44" r:id="rId1" xr:uid="{4A029720-88FF-4614-9FFC-D728903A58CE}"/>
+    <hyperlink ref="D45" r:id="rId1" xr:uid="{4A029720-88FF-4614-9FFC-D728903A58CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Add fields to the excel
</commit_message>
<xml_diff>
--- a/INOW Automation Data Sheet.xlsx
+++ b/INOW Automation Data Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INOW Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\InsuranceNowAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0498D09B-92E1-40A9-825E-5AC8635C260D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831453F3-804F-4291-B098-94E892683A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="17" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="11" activeTab="15" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NewBussines" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6335" uniqueCount="1642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6429" uniqueCount="1696">
   <si>
     <t>NewBussines</t>
   </si>
@@ -4979,6 +4979,168 @@
   </si>
   <si>
     <t>New Business</t>
+  </si>
+  <si>
+    <t>NewCustomerCreation</t>
+  </si>
+  <si>
+    <t>newCustomerEntityType</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualFirst</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualMiddle</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualLast</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualSuffix</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualBirthDate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">newCustomerBypassAddressVerification	</t>
+  </si>
+  <si>
+    <t>newCustomerEntityTypeJoint</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualFirstJoint</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualMiddleJoint</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualLastJoint</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualSuffixJoint</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualBirthDateJoint</t>
+  </si>
+  <si>
+    <t>newCustomerSSNJoint</t>
+  </si>
+  <si>
+    <t>newCustomerBypassAddressVerificationJoint</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualFirst2Joint</t>
+  </si>
+  <si>
+    <t>newCustomerIndividualMiddle2Joint</t>
+  </si>
+  <si>
+    <t>newCustomerPrimaryPhone</t>
+  </si>
+  <si>
+    <t>newCustomerEmail</t>
+  </si>
+  <si>
+    <t>newCustomerFaxNumber</t>
+  </si>
+  <si>
+    <t>newCustomerBestWaytoContact</t>
+  </si>
+  <si>
+    <t>newCustomerBestTimetoContact</t>
+  </si>
+  <si>
+    <t>newCustomerDeliveryPreference</t>
+  </si>
+  <si>
+    <t>newCustomerCustomerNumber</t>
+  </si>
+  <si>
+    <t>NewBusiness_ExistingCustomer</t>
+  </si>
+  <si>
+    <t>existingCustomerSearchBy</t>
+  </si>
+  <si>
+    <t>existingCustomerSearchText</t>
+  </si>
+  <si>
+    <t>existingCustomerEffectiveDt</t>
+  </si>
+  <si>
+    <t>existingCustomerControllingStateCd</t>
+  </si>
+  <si>
+    <t>existingCustomerProgramType</t>
+  </si>
+  <si>
+    <t>existingCustomer</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>09/10/2023</t>
+  </si>
+  <si>
+    <t>Ben</t>
+  </si>
+  <si>
+    <t>Stocks</t>
+  </si>
+  <si>
+    <t>07/09/2000</t>
+  </si>
+  <si>
+    <t>882</t>
+  </si>
+  <si>
+    <t>Individual Address</t>
+  </si>
+  <si>
+    <t>newCustomer</t>
+  </si>
+  <si>
+    <t>newCustomerPrimaryNumber</t>
+  </si>
+  <si>
+    <t>newCustomerStreetName</t>
+  </si>
+  <si>
+    <t>newCustomerCity</t>
+  </si>
+  <si>
+    <t>newCustomerStateProvCd</t>
+  </si>
+  <si>
+    <t>newCustomerPostalCode</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>Wolfforth</t>
+  </si>
+  <si>
+    <t>79382</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>newCustomerPhoneNumber</t>
+  </si>
+  <si>
+    <t>12446678</t>
+  </si>
+  <si>
+    <t>newBusinessHastheinsuredoperatedanuninsuredmotorvehicleformorethan30daysinthepast12months</t>
+  </si>
+  <si>
+    <t>04/02/2017</t>
   </si>
 </sst>
 </file>
@@ -5139,7 +5301,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -5201,6 +5363,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -10045,10 +10210,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA4E5AA-688C-484A-99F1-9AC8F41EC26C}">
-  <dimension ref="A1:D370"/>
+  <dimension ref="A1:D408"/>
   <sheetViews>
-    <sheetView topLeftCell="A365" workbookViewId="0">
-      <selection activeCell="A371" sqref="A371:D371"/>
+    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
+      <selection activeCell="C358" sqref="C358"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10175,15 +10340,17 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="D11" s="1"/>
+        <v>1694</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
@@ -10818,7 +10985,7 @@
         <v>1565</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>1564</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -13723,7 +13890,7 @@
         <v>21</v>
       </c>
       <c r="C358" s="2" t="s">
-        <v>729</v>
+        <v>1586</v>
       </c>
       <c r="D358" s="1" t="s">
         <v>1571</v>
@@ -13849,8 +14016,424 @@
       </c>
       <c r="D370" s="1"/>
     </row>
+    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A371" s="29" t="s">
+        <v>1642</v>
+      </c>
+      <c r="B371" s="29"/>
+      <c r="C371" s="29"/>
+      <c r="D371" s="29"/>
+    </row>
+    <row r="372" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A372" s="1"/>
+      <c r="B372" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C372" s="1" t="s">
+        <v>1643</v>
+      </c>
+      <c r="D372" s="1" t="s">
+        <v>1542</v>
+      </c>
+    </row>
+    <row r="373" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A373" s="1"/>
+      <c r="B373" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C373" s="1" t="s">
+        <v>1644</v>
+      </c>
+      <c r="D373" s="1" t="s">
+        <v>1677</v>
+      </c>
+    </row>
+    <row r="374" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A374" s="1"/>
+      <c r="B374" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C374" s="1" t="s">
+        <v>1645</v>
+      </c>
+      <c r="D374" s="1"/>
+    </row>
+    <row r="375" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A375" s="1"/>
+      <c r="B375" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C375" s="2" t="s">
+        <v>1646</v>
+      </c>
+      <c r="D375" s="1" t="s">
+        <v>1678</v>
+      </c>
+    </row>
+    <row r="376" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A376" s="1"/>
+      <c r="B376" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C376" s="2" t="s">
+        <v>1647</v>
+      </c>
+      <c r="D376" s="1"/>
+    </row>
+    <row r="377" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A377" s="1"/>
+      <c r="B377" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C377" s="2" t="s">
+        <v>1648</v>
+      </c>
+      <c r="D377" s="17" t="s">
+        <v>1679</v>
+      </c>
+    </row>
+    <row r="378" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A378" s="1"/>
+      <c r="B378" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C378" s="1" t="s">
+        <v>1649</v>
+      </c>
+      <c r="D378" s="1"/>
+    </row>
+    <row r="379" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A379" s="1"/>
+      <c r="B379" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C379" s="1" t="s">
+        <v>1650</v>
+      </c>
+      <c r="D379" s="1"/>
+    </row>
+    <row r="380" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A380" s="1"/>
+      <c r="B380" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C380" s="1" t="s">
+        <v>1651</v>
+      </c>
+      <c r="D380" s="1"/>
+    </row>
+    <row r="381" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A381" s="1"/>
+      <c r="B381" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C381" s="1" t="s">
+        <v>1652</v>
+      </c>
+      <c r="D381" s="1"/>
+    </row>
+    <row r="382" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A382" s="1"/>
+      <c r="B382" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C382" s="2" t="s">
+        <v>1653</v>
+      </c>
+      <c r="D382" s="1"/>
+    </row>
+    <row r="383" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A383" s="1"/>
+      <c r="B383" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C383" s="2" t="s">
+        <v>1654</v>
+      </c>
+      <c r="D383" s="1"/>
+    </row>
+    <row r="384" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A384" s="1"/>
+      <c r="B384" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C384" s="2" t="s">
+        <v>1655</v>
+      </c>
+      <c r="D384" s="1"/>
+    </row>
+    <row r="385" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A385" s="1"/>
+      <c r="B385" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C385" s="1" t="s">
+        <v>1656</v>
+      </c>
+      <c r="D385" s="1"/>
+    </row>
+    <row r="386" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A386" s="1"/>
+      <c r="B386" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C386" s="1" t="s">
+        <v>1657</v>
+      </c>
+      <c r="D386" s="1"/>
+    </row>
+    <row r="387" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A387" s="1"/>
+      <c r="B387" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C387" s="1" t="s">
+        <v>1658</v>
+      </c>
+      <c r="D387" s="1"/>
+    </row>
+    <row r="388" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A388" s="1"/>
+      <c r="B388" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C388" s="1" t="s">
+        <v>1659</v>
+      </c>
+      <c r="D388" s="1"/>
+    </row>
+    <row r="389" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A389" s="1"/>
+      <c r="B389" s="2" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C389" s="2" t="s">
+        <v>1683</v>
+      </c>
+      <c r="D389" s="17" t="s">
+        <v>1680</v>
+      </c>
+    </row>
+    <row r="390" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A390" s="1"/>
+      <c r="B390" s="2" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C390" s="2" t="s">
+        <v>1684</v>
+      </c>
+      <c r="D390" s="1" t="s">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="391" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A391" s="1"/>
+      <c r="B391" s="2" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C391" s="2" t="s">
+        <v>1685</v>
+      </c>
+      <c r="D391" s="1" t="s">
+        <v>1689</v>
+      </c>
+    </row>
+    <row r="392" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A392" s="1"/>
+      <c r="B392" s="2" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C392" s="1" t="s">
+        <v>1686</v>
+      </c>
+      <c r="D392" s="1" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="393" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A393" s="1"/>
+      <c r="B393" s="2" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C393" s="1" t="s">
+        <v>1687</v>
+      </c>
+      <c r="D393" s="17" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="394" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A394" s="1"/>
+      <c r="B394" s="2" t="s">
+        <v>1681</v>
+      </c>
+      <c r="C394" s="1" t="s">
+        <v>1682</v>
+      </c>
+      <c r="D394" s="1"/>
+    </row>
+    <row r="395" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A395" s="1"/>
+      <c r="B395" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C395" s="1" t="s">
+        <v>1660</v>
+      </c>
+      <c r="D395" s="1" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+    <row r="396" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A396" s="1"/>
+      <c r="B396" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C396" s="1" t="s">
+        <v>1692</v>
+      </c>
+      <c r="D396" s="17" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="397" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A397" s="1"/>
+      <c r="B397" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C397" s="5" t="s">
+        <v>1661</v>
+      </c>
+      <c r="D397" s="1" t="s">
+        <v>1548</v>
+      </c>
+    </row>
+    <row r="398" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A398" s="1"/>
+      <c r="B398" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C398" s="1" t="s">
+        <v>1662</v>
+      </c>
+      <c r="D398" s="1"/>
+    </row>
+    <row r="399" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A399" s="1"/>
+      <c r="B399" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C399" s="1" t="s">
+        <v>1663</v>
+      </c>
+      <c r="D399" s="1" t="s">
+        <v>1543</v>
+      </c>
+    </row>
+    <row r="400" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A400" s="1"/>
+      <c r="B400" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C400" s="1" t="s">
+        <v>1664</v>
+      </c>
+      <c r="D400" s="1" t="s">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="401" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A401" s="1"/>
+      <c r="B401" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C401" s="1" t="s">
+        <v>1665</v>
+      </c>
+      <c r="D401" s="1"/>
+    </row>
+    <row r="402" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A402" s="1"/>
+      <c r="B402" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C402" s="1" t="s">
+        <v>1666</v>
+      </c>
+      <c r="D402" s="1"/>
+    </row>
+    <row r="403" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A403" s="29" t="s">
+        <v>1667</v>
+      </c>
+      <c r="B403" s="29"/>
+      <c r="C403" s="29"/>
+      <c r="D403" s="29"/>
+    </row>
+    <row r="404" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A404" s="1"/>
+      <c r="B404" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C404" s="13" t="s">
+        <v>1668</v>
+      </c>
+      <c r="D404" s="1" t="s">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="405" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A405" s="1"/>
+      <c r="B405" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C405" s="13" t="s">
+        <v>1669</v>
+      </c>
+      <c r="D405" s="17" t="s">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="406" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A406" s="1"/>
+      <c r="B406" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C406" s="13" t="s">
+        <v>1670</v>
+      </c>
+      <c r="D406" s="17" t="s">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="407" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A407" s="1"/>
+      <c r="B407" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C407" s="13" t="s">
+        <v>1671</v>
+      </c>
+      <c r="D407" s="1" t="s">
+        <v>1536</v>
+      </c>
+    </row>
+    <row r="408" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A408" s="1"/>
+      <c r="B408" s="1" t="s">
+        <v>1673</v>
+      </c>
+      <c r="C408" s="13" t="s">
+        <v>1672</v>
+      </c>
+      <c r="D408" s="1" t="s">
+        <v>1537</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="10">
+    <mergeCell ref="A371:D371"/>
+    <mergeCell ref="A403:D403"/>
     <mergeCell ref="A278:A331"/>
     <mergeCell ref="A332:A353"/>
     <mergeCell ref="A1:D1"/>
@@ -13872,7 +14455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE3BCC8-1641-433F-8FC0-0BC9EA113D75}">
   <dimension ref="D1:G736"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
@@ -21362,6 +21945,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D174:D277"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D3:D49"/>
+    <mergeCell ref="D50:D59"/>
+    <mergeCell ref="D60:D157"/>
+    <mergeCell ref="D158:D173"/>
     <mergeCell ref="D524:D539"/>
     <mergeCell ref="D540:D643"/>
     <mergeCell ref="D644:D697"/>
@@ -21372,12 +21961,6 @@
     <mergeCell ref="D373:D415"/>
     <mergeCell ref="D416:D425"/>
     <mergeCell ref="D426:D523"/>
-    <mergeCell ref="D174:D277"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D3:D49"/>
-    <mergeCell ref="D50:D59"/>
-    <mergeCell ref="D60:D157"/>
-    <mergeCell ref="D158:D173"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G44" r:id="rId1" xr:uid="{249BC4C0-3423-4E91-A0D7-112396468B55}"/>
@@ -21390,8 +21973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC48D60B-A2DA-4B33-8870-4BC720D13BF5}">
   <dimension ref="A1:D416"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="A1:D416"/>
+    <sheetView topLeftCell="A356" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25692,18 +26275,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A371:D371"/>
+    <mergeCell ref="A381:D381"/>
+    <mergeCell ref="A391:D391"/>
+    <mergeCell ref="A403:D403"/>
+    <mergeCell ref="A278:A331"/>
+    <mergeCell ref="A332:A353"/>
     <mergeCell ref="A174:A277"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:A49"/>
     <mergeCell ref="A50:A59"/>
     <mergeCell ref="A60:A157"/>
     <mergeCell ref="A158:A173"/>
-    <mergeCell ref="A371:D371"/>
-    <mergeCell ref="A381:D381"/>
-    <mergeCell ref="A391:D391"/>
-    <mergeCell ref="A403:D403"/>
-    <mergeCell ref="A278:A331"/>
-    <mergeCell ref="A332:A353"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D44" r:id="rId1" xr:uid="{DE8D0F4F-6169-48C2-82D8-7C8293E1696B}"/>

</xml_diff>

<commit_message>
updates of excel sheet(removal of gaps in endorsement non driver labels)
</commit_message>
<xml_diff>
--- a/INOW Automation Data Sheet.xlsx
+++ b/INOW Automation Data Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InsuranceNowAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ABA827-2614-41F0-8CB8-811A07162F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AEE311-CAFF-4114-9353-2E5CAD12CA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="16" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6404" uniqueCount="1680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6404" uniqueCount="1688">
   <si>
     <t>NewBussines</t>
   </si>
@@ -5093,6 +5093,30 @@
   </si>
   <si>
     <t>19XFC1F36GE218891</t>
+  </si>
+  <si>
+    <t>endorsementNonDriver1LastName</t>
+  </si>
+  <si>
+    <t>endorsementNonDriver1RelationshipToInsured</t>
+  </si>
+  <si>
+    <t>endorsementNonDriver1NonDriverType</t>
+  </si>
+  <si>
+    <t>endorsementNonDriver1Gender</t>
+  </si>
+  <si>
+    <t>endorsementNonDriver2MiddleName</t>
+  </si>
+  <si>
+    <t>endorsementNonDriver2LastName</t>
+  </si>
+  <si>
+    <t>endorsementNonDriver2NonDriverType</t>
+  </si>
+  <si>
+    <t>endorsementNonDriver2Gender</t>
   </si>
 </sst>
 </file>
@@ -14245,8 +14269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE3BCC8-1641-433F-8FC0-0BC9EA113D75}">
   <dimension ref="D1:G736"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A541" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H550" sqref="H550"/>
+    <sheetView tabSelected="1" topLeftCell="A525" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F539" sqref="F539"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19603,7 +19627,7 @@
         <v>15</v>
       </c>
       <c r="F526" s="1" t="s">
-        <v>161</v>
+        <v>1680</v>
       </c>
       <c r="G526" s="1" t="s">
         <v>1594</v>
@@ -19615,7 +19639,7 @@
         <v>15</v>
       </c>
       <c r="F527" s="1" t="s">
-        <v>162</v>
+        <v>1681</v>
       </c>
       <c r="G527" s="1" t="s">
         <v>1595</v>
@@ -19627,7 +19651,7 @@
         <v>15</v>
       </c>
       <c r="F528" s="1" t="s">
-        <v>163</v>
+        <v>1682</v>
       </c>
       <c r="G528" s="1" t="s">
         <v>1605</v>
@@ -19639,7 +19663,7 @@
         <v>15</v>
       </c>
       <c r="F529" s="1" t="s">
-        <v>164</v>
+        <v>1683</v>
       </c>
       <c r="G529" s="1" t="s">
         <v>1558</v>
@@ -19687,7 +19711,7 @@
         <v>15</v>
       </c>
       <c r="F533" s="1" t="s">
-        <v>168</v>
+        <v>1684</v>
       </c>
       <c r="G533" s="1"/>
     </row>
@@ -19697,7 +19721,7 @@
         <v>15</v>
       </c>
       <c r="F534" s="1" t="s">
-        <v>169</v>
+        <v>1685</v>
       </c>
       <c r="G534" s="1" t="s">
         <v>1599</v>
@@ -19721,7 +19745,7 @@
         <v>15</v>
       </c>
       <c r="F536" s="1" t="s">
-        <v>171</v>
+        <v>1686</v>
       </c>
       <c r="G536" s="1" t="s">
         <v>1605</v>
@@ -19733,7 +19757,7 @@
         <v>15</v>
       </c>
       <c r="F537" s="1" t="s">
-        <v>172</v>
+        <v>1687</v>
       </c>
       <c r="G537" s="1" t="s">
         <v>1601</v>
@@ -21751,6 +21775,12 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D174:D277"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D3:D49"/>
+    <mergeCell ref="D50:D59"/>
+    <mergeCell ref="D60:D157"/>
+    <mergeCell ref="D158:D173"/>
     <mergeCell ref="D524:D539"/>
     <mergeCell ref="D540:D643"/>
     <mergeCell ref="D644:D697"/>
@@ -21761,17 +21791,12 @@
     <mergeCell ref="D373:D415"/>
     <mergeCell ref="D416:D425"/>
     <mergeCell ref="D426:D523"/>
-    <mergeCell ref="D174:D277"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D3:D49"/>
-    <mergeCell ref="D50:D59"/>
-    <mergeCell ref="D60:D157"/>
-    <mergeCell ref="D158:D173"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G44" r:id="rId1" xr:uid="{249BC4C0-3423-4E91-A0D7-112396468B55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -26081,18 +26106,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A371:D371"/>
+    <mergeCell ref="A381:D381"/>
+    <mergeCell ref="A391:D391"/>
+    <mergeCell ref="A403:D403"/>
+    <mergeCell ref="A278:A331"/>
+    <mergeCell ref="A332:A353"/>
     <mergeCell ref="A174:A277"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:A49"/>
     <mergeCell ref="A50:A59"/>
     <mergeCell ref="A60:A157"/>
     <mergeCell ref="A158:A173"/>
-    <mergeCell ref="A371:D371"/>
-    <mergeCell ref="A381:D381"/>
-    <mergeCell ref="A391:D391"/>
-    <mergeCell ref="A403:D403"/>
-    <mergeCell ref="A278:A331"/>
-    <mergeCell ref="A332:A353"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D44" r:id="rId1" xr:uid="{DE8D0F4F-6169-48C2-82D8-7C8293E1696B}"/>

</xml_diff>

<commit_message>
procer class added to excel
</commit_message>
<xml_diff>
--- a/INOW Automation Data Sheet.xlsx
+++ b/INOW Automation Data Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INOW Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InsuranceNowAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5C9452-8237-48DE-9AC4-BB7A734B828F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ABA827-2614-41F0-8CB8-811A07162F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="12" activeTab="18" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="16" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NewBussines" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <sheet name="TS_01" sheetId="25" r:id="rId16"/>
     <sheet name="TS_02" sheetId="28" r:id="rId17"/>
     <sheet name="TS_03" sheetId="29" r:id="rId18"/>
-    <sheet name="Producer" sheetId="32" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6558" uniqueCount="1762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6404" uniqueCount="1680">
   <si>
     <t>NewBussines</t>
   </si>
@@ -5094,252 +5093,6 @@
   </si>
   <si>
     <t>19XFC1F36GE218891</t>
-  </si>
-  <si>
-    <t>Producer</t>
-  </si>
-  <si>
-    <t>Producer Detail</t>
-  </si>
-  <si>
-    <t>producerCode</t>
-  </si>
-  <si>
-    <t>producerType</t>
-  </si>
-  <si>
-    <t>producerAgency</t>
-  </si>
-  <si>
-    <t>producerGroup</t>
-  </si>
-  <si>
-    <t>producerStatus</t>
-  </si>
-  <si>
-    <t>producerStatusDate</t>
-  </si>
-  <si>
-    <t>producerDateAppointed</t>
-  </si>
-  <si>
-    <t>producerBusinessType</t>
-  </si>
-  <si>
-    <t>producerName</t>
-  </si>
-  <si>
-    <t>producerBusinessName</t>
-  </si>
-  <si>
-    <t>producerSearchName</t>
-  </si>
-  <si>
-    <t>producerDBA</t>
-  </si>
-  <si>
-    <t>producerSearchDBA</t>
-  </si>
-  <si>
-    <t>producerAddress</t>
-  </si>
-  <si>
-    <t>producerCity</t>
-  </si>
-  <si>
-    <t>producerZip</t>
-  </si>
-  <si>
-    <t>producerCountry</t>
-  </si>
-  <si>
-    <t>Street Address</t>
-  </si>
-  <si>
-    <t>Billing Address</t>
-  </si>
-  <si>
-    <t>producerBillingAddress</t>
-  </si>
-  <si>
-    <t>producerBillingCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">producerBillingState </t>
-  </si>
-  <si>
-    <t>producerBillingZip</t>
-  </si>
-  <si>
-    <t>producerBillingCountry</t>
-  </si>
-  <si>
-    <t>producerPrimaryPhone</t>
-  </si>
-  <si>
-    <t>producerSecondaryPhone</t>
-  </si>
-  <si>
-    <t>producerFaxNumber</t>
-  </si>
-  <si>
-    <t>producerEmailAddress</t>
-  </si>
-  <si>
-    <t>producerDeliveryPreference</t>
-  </si>
-  <si>
-    <t>producerEOCarrier</t>
-  </si>
-  <si>
-    <t>producerEOPolicyNumber</t>
-  </si>
-  <si>
-    <t>producerEOExpirationDate</t>
-  </si>
-  <si>
-    <t>producerBranchCode</t>
-  </si>
-  <si>
-    <t>producerReplacedbyProducer</t>
-  </si>
-  <si>
-    <t>producerReplacedbyEffDate</t>
-  </si>
-  <si>
-    <t>producerSubmitToUser</t>
-  </si>
-  <si>
-    <t>producerSubmitToGroup</t>
-  </si>
-  <si>
-    <t>producerDirectPortal</t>
-  </si>
-  <si>
-    <t>producereSignatureMethod</t>
-  </si>
-  <si>
-    <t>producerAgencyRenewalFee</t>
-  </si>
-  <si>
-    <t>producereSignature</t>
-  </si>
-  <si>
-    <t>Accounting Information</t>
-  </si>
-  <si>
-    <t>producerAccountingEntityName</t>
-  </si>
-  <si>
-    <t>producerPayTo</t>
-  </si>
-  <si>
-    <t>producerAccountEntryType</t>
-  </si>
-  <si>
-    <t>producerAccountType</t>
-  </si>
-  <si>
-    <t>producerAllowCombinedPayments</t>
-  </si>
-  <si>
-    <t>producerBankName</t>
-  </si>
-  <si>
-    <t>producerPaymentBy</t>
-  </si>
-  <si>
-    <t>producerAccountNumber</t>
-  </si>
-  <si>
-    <t>producerRoutingNumber</t>
-  </si>
-  <si>
-    <t>producerMailingAddress</t>
-  </si>
-  <si>
-    <t>producerMailingCity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">producerMailingState </t>
-  </si>
-  <si>
-    <t>producerMailingZip</t>
-  </si>
-  <si>
-    <t>producerMailingCountry</t>
-  </si>
-  <si>
-    <t>State Detail</t>
-  </si>
-  <si>
-    <t>producerStateDetail</t>
-  </si>
-  <si>
-    <t>Licensed Product Class List</t>
-  </si>
-  <si>
-    <t>producerLicensedState</t>
-  </si>
-  <si>
-    <t>producerLicensedProgramType</t>
-  </si>
-  <si>
-    <t>producerLicensedLicenseClassCode</t>
-  </si>
-  <si>
-    <t>producerLicensedChannel</t>
-  </si>
-  <si>
-    <t>producerLicensedEffectivDate</t>
-  </si>
-  <si>
-    <t>producerLicensedCommissionNB</t>
-  </si>
-  <si>
-    <t>producerLicensedCommissionOther</t>
-  </si>
-  <si>
-    <t>producerLicensedNBExpDate</t>
-  </si>
-  <si>
-    <t>producerLicensedRnwlExpDate</t>
-  </si>
-  <si>
-    <t>producerLicensedSubmitToUser</t>
-  </si>
-  <si>
-    <t>producerLicensedSubmitToGroup</t>
-  </si>
-  <si>
-    <t>producerLicensedCommissionPaidOut</t>
-  </si>
-  <si>
-    <t>producerLicensedCommissionPayRule</t>
-  </si>
-  <si>
-    <t>producerLicensedExpirationDate</t>
-  </si>
-  <si>
-    <t>producerState</t>
-  </si>
-  <si>
-    <t>producerEOLimit</t>
-  </si>
-  <si>
-    <t>producerLastCommissionPayThroughDate</t>
-  </si>
-  <si>
-    <t>producerStateProgramType</t>
-  </si>
-  <si>
-    <t>producerStateDateAppointed</t>
-  </si>
-  <si>
-    <t>producerStateDateCancelled</t>
-  </si>
-  <si>
-    <t>producerLicensedCommissionRenewal</t>
   </si>
 </sst>
 </file>
@@ -5411,7 +5164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -5495,36 +5248,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -5588,18 +5317,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -10106,7 +9823,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14528,7 +14245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE3BCC8-1641-433F-8FC0-0BC9EA113D75}">
   <dimension ref="D1:G736"/>
   <sheetViews>
-    <sheetView topLeftCell="A541" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A541" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H550" sqref="H550"/>
     </sheetView>
   </sheetViews>
@@ -22034,12 +21751,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D174:D277"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D3:D49"/>
-    <mergeCell ref="D50:D59"/>
-    <mergeCell ref="D60:D157"/>
-    <mergeCell ref="D158:D173"/>
     <mergeCell ref="D524:D539"/>
     <mergeCell ref="D540:D643"/>
     <mergeCell ref="D644:D697"/>
@@ -22050,6 +21761,12 @@
     <mergeCell ref="D373:D415"/>
     <mergeCell ref="D416:D425"/>
     <mergeCell ref="D426:D523"/>
+    <mergeCell ref="D174:D277"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D3:D49"/>
+    <mergeCell ref="D50:D59"/>
+    <mergeCell ref="D60:D157"/>
+    <mergeCell ref="D158:D173"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G44" r:id="rId1" xr:uid="{249BC4C0-3423-4E91-A0D7-112396468B55}"/>
@@ -22062,7 +21779,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC48D60B-A2DA-4B33-8870-4BC720D13BF5}">
   <dimension ref="A1:D416"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A380" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -26364,685 +26081,23 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A174:A277"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A49"/>
+    <mergeCell ref="A50:A59"/>
+    <mergeCell ref="A60:A157"/>
+    <mergeCell ref="A158:A173"/>
     <mergeCell ref="A371:D371"/>
     <mergeCell ref="A381:D381"/>
     <mergeCell ref="A391:D391"/>
     <mergeCell ref="A403:D403"/>
     <mergeCell ref="A278:A331"/>
     <mergeCell ref="A332:A353"/>
-    <mergeCell ref="A174:A277"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A49"/>
-    <mergeCell ref="A50:A59"/>
-    <mergeCell ref="A60:A157"/>
-    <mergeCell ref="A158:A173"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D44" r:id="rId1" xr:uid="{DE8D0F4F-6169-48C2-82D8-7C8293E1696B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C04EFC45-3CE5-45C4-B440-20040531B5D8}">
-  <dimension ref="A1:C83"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C76" sqref="C76"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="46.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="39.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="48.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="35.28515625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
-        <v>1680</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="34"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>1682</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>1683</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>1685</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1686</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1687</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>1688</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>1689</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>1690</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>1691</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>1692</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>1693</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>1681</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>1695</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>1696</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1755</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>1697</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>1699</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>1698</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>1701</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>1703</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>1704</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>1700</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>1705</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>1706</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>1707</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>1708</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>1709</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>1710</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>1711</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>1712</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>1756</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>1713</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>1714</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>1715</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>1716</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>1717</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>1718</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>1719</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>1720</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>1721</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>1722</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" s="31" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>1724</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" s="31" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>1725</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" s="31" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" s="31" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>1727</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="31" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>1728</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="31" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>1729</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="31" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="31" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>1731</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="31" t="s">
-        <v>1723</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>1732</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>1733</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>1734</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>1735</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>1736</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>1737</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>1739</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="2" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>1758</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>1759</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>1760</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>1738</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>1754</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>1741</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>1742</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>1743</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>1744</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>1745</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>1746</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>1761</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>1747</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>1748</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>1749</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>1751</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>1752</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="2" t="s">
-        <v>1740</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>1753</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="2"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="2"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="2"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="2"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="2"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="2"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Endorsement label gaps removals
</commit_message>
<xml_diff>
--- a/INOW Automation Data Sheet.xlsx
+++ b/INOW Automation Data Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InsuranceNowAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AEE311-CAFF-4114-9353-2E5CAD12CA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3E5255-B20C-4B74-8E89-D8173689457B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="16" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6404" uniqueCount="1688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6405" uniqueCount="1691">
   <si>
     <t>NewBussines</t>
   </si>
@@ -5117,6 +5117,15 @@
   </si>
   <si>
     <t>endorsementNonDriver2Gender</t>
+  </si>
+  <si>
+    <t>endorsementNonDriver2RelationshipToInsured</t>
+  </si>
+  <si>
+    <t>endorsementVehicle1PurchasedOrLeased</t>
+  </si>
+  <si>
+    <t>endorsementVehicle1TowingAndLabor</t>
   </si>
 </sst>
 </file>
@@ -14269,8 +14278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE3BCC8-1641-433F-8FC0-0BC9EA113D75}">
   <dimension ref="D1:G736"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A525" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F539" sqref="F539"/>
+    <sheetView tabSelected="1" topLeftCell="A718" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F722" sqref="F722"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19733,7 +19742,7 @@
         <v>15</v>
       </c>
       <c r="F535" s="1" t="s">
-        <v>170</v>
+        <v>1688</v>
       </c>
       <c r="G535" s="1" t="s">
         <v>1600</v>
@@ -19783,7 +19792,9 @@
       <c r="F539" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G539" s="1"/>
+      <c r="G539" s="1" t="s">
+        <v>1597</v>
+      </c>
     </row>
     <row r="540" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D540" s="23" t="s">
@@ -19907,7 +19918,7 @@
         <v>16</v>
       </c>
       <c r="F551" s="1" t="s">
-        <v>186</v>
+        <v>1689</v>
       </c>
       <c r="G551" s="1" t="s">
         <v>1569</v>
@@ -20005,7 +20016,7 @@
         <v>16</v>
       </c>
       <c r="F560" s="1" t="s">
-        <v>195</v>
+        <v>1690</v>
       </c>
       <c r="G560" s="1" t="s">
         <v>1571</v>

</xml_diff>

<commit_message>
producer code VO class Update
</commit_message>
<xml_diff>
--- a/INOW Automation Data Sheet.xlsx
+++ b/INOW Automation Data Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\INOW Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InsuranceNowAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34056C6C-0EF0-4428-82F2-A63ABDB3FAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08ABA827-2614-41F0-8CB8-811A07162F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="13" activeTab="18" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="16" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NewBussines" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,6 @@
     <sheet name="TS_01" sheetId="25" r:id="rId16"/>
     <sheet name="TS_02" sheetId="28" r:id="rId17"/>
     <sheet name="TS_03" sheetId="29" r:id="rId18"/>
-    <sheet name="Producer Creation" sheetId="32" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6558" uniqueCount="1761">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6404" uniqueCount="1680">
   <si>
     <t>NewBussines</t>
   </si>
@@ -5094,249 +5093,6 @@
   </si>
   <si>
     <t>19XFC1F36GE218891</t>
-  </si>
-  <si>
-    <t>producerCode</t>
-  </si>
-  <si>
-    <t>producerType</t>
-  </si>
-  <si>
-    <t>producerStatus</t>
-  </si>
-  <si>
-    <t>producerAgency</t>
-  </si>
-  <si>
-    <t>producerGroup</t>
-  </si>
-  <si>
-    <t>producerStatusDate</t>
-  </si>
-  <si>
-    <t>producerDateAppointed</t>
-  </si>
-  <si>
-    <t>producerBusinessType</t>
-  </si>
-  <si>
-    <t>producerName</t>
-  </si>
-  <si>
-    <t>producerBusinessName</t>
-  </si>
-  <si>
-    <t>producerSearchName</t>
-  </si>
-  <si>
-    <t>producerDBA</t>
-  </si>
-  <si>
-    <t>producerSearchDBA</t>
-  </si>
-  <si>
-    <t>producerAddress</t>
-  </si>
-  <si>
-    <t>producerCity</t>
-  </si>
-  <si>
-    <t>producerState</t>
-  </si>
-  <si>
-    <t>producerZip</t>
-  </si>
-  <si>
-    <t>producerCountry</t>
-  </si>
-  <si>
-    <t>producerBillingAddress</t>
-  </si>
-  <si>
-    <t>producerBillingCity</t>
-  </si>
-  <si>
-    <t>producerBillingState</t>
-  </si>
-  <si>
-    <t>producerBillingZip</t>
-  </si>
-  <si>
-    <t>producerBillingCountry</t>
-  </si>
-  <si>
-    <t>producerPrimaryPhone</t>
-  </si>
-  <si>
-    <t>producerSecondaryPhone</t>
-  </si>
-  <si>
-    <t>producerFaxNumber</t>
-  </si>
-  <si>
-    <t>producerEmailAddress</t>
-  </si>
-  <si>
-    <t>producerDeliveryPreference</t>
-  </si>
-  <si>
-    <t>producerEOCarrier</t>
-  </si>
-  <si>
-    <t>producerEOPolicyNumber</t>
-  </si>
-  <si>
-    <t>producerEOLimit</t>
-  </si>
-  <si>
-    <t>producerEOExpirationDate</t>
-  </si>
-  <si>
-    <t>producerBranchCode</t>
-  </si>
-  <si>
-    <t>producerReplacedbyProducer</t>
-  </si>
-  <si>
-    <t>producerReplacedbyEffDate</t>
-  </si>
-  <si>
-    <t>producerSubmitToUser</t>
-  </si>
-  <si>
-    <t>producerSubmitToGroup</t>
-  </si>
-  <si>
-    <t>producerLastCommissionPayThroughDate</t>
-  </si>
-  <si>
-    <t>producerDirectPortal</t>
-  </si>
-  <si>
-    <t>producereSignatureMethod</t>
-  </si>
-  <si>
-    <t>producerAgencyRenewalFee</t>
-  </si>
-  <si>
-    <t>producereSignature</t>
-  </si>
-  <si>
-    <t>producerAccountingEntityName</t>
-  </si>
-  <si>
-    <t>producerPayTo</t>
-  </si>
-  <si>
-    <t>producerAccountEntryType</t>
-  </si>
-  <si>
-    <t>producerAccountType</t>
-  </si>
-  <si>
-    <t>producerAllowCombinedPayments</t>
-  </si>
-  <si>
-    <t>producerBankName</t>
-  </si>
-  <si>
-    <t>producerPaymentBy</t>
-  </si>
-  <si>
-    <t>producerAccountNumber</t>
-  </si>
-  <si>
-    <t>producerRoutingNumber</t>
-  </si>
-  <si>
-    <t>producerMailingAddress</t>
-  </si>
-  <si>
-    <t>producerMailingCity</t>
-  </si>
-  <si>
-    <t>producerMailingState</t>
-  </si>
-  <si>
-    <t>producerMailingZip</t>
-  </si>
-  <si>
-    <t>producerMailingCountry</t>
-  </si>
-  <si>
-    <t>producerStateDetail</t>
-  </si>
-  <si>
-    <t>producerStateProgramType</t>
-  </si>
-  <si>
-    <t>producerStateDateAppointed</t>
-  </si>
-  <si>
-    <t>producerStateDateCancelled</t>
-  </si>
-  <si>
-    <t>producerLicensedExpirationDate</t>
-  </si>
-  <si>
-    <t>producerLicensedState</t>
-  </si>
-  <si>
-    <t>producerLicensedProgramType</t>
-  </si>
-  <si>
-    <t>producerLicensedLicenseClassCode</t>
-  </si>
-  <si>
-    <t>producerLicensedChannel</t>
-  </si>
-  <si>
-    <t>producerLicensedEffectivDate</t>
-  </si>
-  <si>
-    <t>producerLicensedCommissionNB</t>
-  </si>
-  <si>
-    <t>producerLicensedCommissionRenewal</t>
-  </si>
-  <si>
-    <t>producerLicensedCommissionOther</t>
-  </si>
-  <si>
-    <t>producerLicensedNBExpDate</t>
-  </si>
-  <si>
-    <t>producerLicensedRnwlExpDate</t>
-  </si>
-  <si>
-    <t>producerLicensedSubmitToUser</t>
-  </si>
-  <si>
-    <t>producerLicensedSubmitToGroup</t>
-  </si>
-  <si>
-    <t>producerLicensedCommissionPaidOut</t>
-  </si>
-  <si>
-    <t>producerLicensedCommissionPayRule</t>
-  </si>
-  <si>
-    <t>Producer Detail</t>
-  </si>
-  <si>
-    <t>Street Address</t>
-  </si>
-  <si>
-    <t>Billing Address</t>
-  </si>
-  <si>
-    <t>Accounting Information</t>
-  </si>
-  <si>
-    <t>State Detail</t>
-  </si>
-  <si>
-    <t>Licensed Product Class List</t>
   </si>
 </sst>
 </file>
@@ -5346,7 +5102,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5381,19 +5137,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF080808"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -5421,7 +5164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -5505,36 +5248,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -5599,33 +5318,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -14553,7 +14245,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE3BCC8-1641-433F-8FC0-0BC9EA113D75}">
   <dimension ref="D1:G736"/>
   <sheetViews>
-    <sheetView topLeftCell="A541" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A541" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H550" sqref="H550"/>
     </sheetView>
   </sheetViews>
@@ -22059,12 +21751,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D174:D277"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D3:D49"/>
-    <mergeCell ref="D50:D59"/>
-    <mergeCell ref="D60:D157"/>
-    <mergeCell ref="D158:D173"/>
     <mergeCell ref="D524:D539"/>
     <mergeCell ref="D540:D643"/>
     <mergeCell ref="D644:D697"/>
@@ -22075,6 +21761,12 @@
     <mergeCell ref="D373:D415"/>
     <mergeCell ref="D416:D425"/>
     <mergeCell ref="D426:D523"/>
+    <mergeCell ref="D174:D277"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D3:D49"/>
+    <mergeCell ref="D50:D59"/>
+    <mergeCell ref="D60:D157"/>
+    <mergeCell ref="D158:D173"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G44" r:id="rId1" xr:uid="{249BC4C0-3423-4E91-A0D7-112396468B55}"/>
@@ -22087,8 +21779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC48D60B-A2DA-4B33-8870-4BC720D13BF5}">
   <dimension ref="A1:D416"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+    <sheetView topLeftCell="A380" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26389,816 +26081,22 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A174:A277"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A49"/>
+    <mergeCell ref="A50:A59"/>
+    <mergeCell ref="A60:A157"/>
+    <mergeCell ref="A158:A173"/>
     <mergeCell ref="A371:D371"/>
     <mergeCell ref="A381:D381"/>
     <mergeCell ref="A391:D391"/>
     <mergeCell ref="A403:D403"/>
     <mergeCell ref="A278:A331"/>
     <mergeCell ref="A332:A353"/>
-    <mergeCell ref="A174:A277"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A49"/>
-    <mergeCell ref="A50:A59"/>
-    <mergeCell ref="A60:A157"/>
-    <mergeCell ref="A158:A173"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D44" r:id="rId1" xr:uid="{DE8D0F4F-6169-48C2-82D8-7C8293E1696B}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91F57D5C-24F6-45DD-BB48-DD69252BEB36}">
-  <dimension ref="A1:D77"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.140625" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>1641</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="33"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="34" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="35"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B3" s="36" t="s">
-        <v>1680</v>
-      </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>1681</v>
-      </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>1683</v>
-      </c>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B6" s="36" t="s">
-        <v>1684</v>
-      </c>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>1682</v>
-      </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B8" s="36" t="s">
-        <v>1685</v>
-      </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>1686</v>
-      </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>1687</v>
-      </c>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>1688</v>
-      </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B12" s="36" t="s">
-        <v>1689</v>
-      </c>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B13" s="36" t="s">
-        <v>1690</v>
-      </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B14" s="36" t="s">
-        <v>1691</v>
-      </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="35" t="s">
-        <v>1755</v>
-      </c>
-      <c r="B15" s="36" t="s">
-        <v>1692</v>
-      </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="35" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>1693</v>
-      </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="35" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>1694</v>
-      </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="35" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B18" s="36" t="s">
-        <v>1695</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>1696</v>
-      </c>
-      <c r="C19" s="35"/>
-      <c r="D19" s="35"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="35" t="s">
-        <v>1756</v>
-      </c>
-      <c r="B20" s="37" t="s">
-        <v>1697</v>
-      </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="35" t="s">
-        <v>1757</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>1698</v>
-      </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="35" t="s">
-        <v>1757</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>1699</v>
-      </c>
-      <c r="C22" s="35"/>
-      <c r="D22" s="35"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="35" t="s">
-        <v>1757</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>1700</v>
-      </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="35" t="s">
-        <v>1757</v>
-      </c>
-      <c r="B24" s="37" t="s">
-        <v>1701</v>
-      </c>
-      <c r="C24" s="35"/>
-      <c r="D24" s="35"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="35" t="s">
-        <v>1757</v>
-      </c>
-      <c r="B25" s="37" t="s">
-        <v>1702</v>
-      </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="35"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B26" s="37" t="s">
-        <v>1703</v>
-      </c>
-      <c r="C26" s="35"/>
-      <c r="D26" s="35"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="37" t="s">
-        <v>1704</v>
-      </c>
-      <c r="C27" s="35"/>
-      <c r="D27" s="35"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="37" t="s">
-        <v>1705</v>
-      </c>
-      <c r="C28" s="35"/>
-      <c r="D28" s="35"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="37" t="s">
-        <v>1706</v>
-      </c>
-      <c r="C29" s="35"/>
-      <c r="D29" s="35"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B30" s="37" t="s">
-        <v>1707</v>
-      </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="35"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="37" t="s">
-        <v>1708</v>
-      </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="35"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B32" s="37" t="s">
-        <v>1709</v>
-      </c>
-      <c r="C32" s="35"/>
-      <c r="D32" s="35"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="37" t="s">
-        <v>1710</v>
-      </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="35"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B34" s="37" t="s">
-        <v>1711</v>
-      </c>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B35" s="37" t="s">
-        <v>1712</v>
-      </c>
-      <c r="C35" s="35"/>
-      <c r="D35" s="35"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="37" t="s">
-        <v>1713</v>
-      </c>
-      <c r="C36" s="35"/>
-      <c r="D36" s="35"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B37" s="37" t="s">
-        <v>1714</v>
-      </c>
-      <c r="C37" s="35"/>
-      <c r="D37" s="35"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B38" s="37" t="s">
-        <v>1715</v>
-      </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="35"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" s="37" t="s">
-        <v>1716</v>
-      </c>
-      <c r="C39" s="35"/>
-      <c r="D39" s="35"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="37" t="s">
-        <v>1717</v>
-      </c>
-      <c r="C40" s="35"/>
-      <c r="D40" s="35"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B41" s="37" t="s">
-        <v>1718</v>
-      </c>
-      <c r="C41" s="35"/>
-      <c r="D41" s="35"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="37" t="s">
-        <v>1719</v>
-      </c>
-      <c r="C42" s="35"/>
-      <c r="D42" s="35"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B43" s="37" t="s">
-        <v>1720</v>
-      </c>
-      <c r="C43" s="35"/>
-      <c r="D43" s="35"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="36" t="s">
-        <v>9</v>
-      </c>
-      <c r="B44" s="37" t="s">
-        <v>1721</v>
-      </c>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="36" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B45" s="37" t="s">
-        <v>1722</v>
-      </c>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="36" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B46" s="37" t="s">
-        <v>1723</v>
-      </c>
-      <c r="C46" s="35"/>
-      <c r="D46" s="35"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="36" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B47" s="37" t="s">
-        <v>1724</v>
-      </c>
-      <c r="C47" s="35"/>
-      <c r="D47" s="35"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="36" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B48" s="37" t="s">
-        <v>1725</v>
-      </c>
-      <c r="C48" s="35"/>
-      <c r="D48" s="35"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="36" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B49" s="37" t="s">
-        <v>1726</v>
-      </c>
-      <c r="C49" s="35"/>
-      <c r="D49" s="35"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="36" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B50" s="37" t="s">
-        <v>1727</v>
-      </c>
-      <c r="C50" s="35"/>
-      <c r="D50" s="35"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="36" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B51" s="37" t="s">
-        <v>1728</v>
-      </c>
-      <c r="C51" s="35"/>
-      <c r="D51" s="35"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="36" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B52" s="37" t="s">
-        <v>1729</v>
-      </c>
-      <c r="C52" s="35"/>
-      <c r="D52" s="35"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="36" t="s">
-        <v>1758</v>
-      </c>
-      <c r="B53" s="37" t="s">
-        <v>1730</v>
-      </c>
-      <c r="C53" s="35"/>
-      <c r="D53" s="35"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B54" s="37" t="s">
-        <v>1731</v>
-      </c>
-      <c r="C54" s="35"/>
-      <c r="D54" s="35"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B55" s="37" t="s">
-        <v>1732</v>
-      </c>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B56" s="37" t="s">
-        <v>1733</v>
-      </c>
-      <c r="C56" s="35"/>
-      <c r="D56" s="35"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B57" s="37" t="s">
-        <v>1734</v>
-      </c>
-      <c r="C57" s="35"/>
-      <c r="D57" s="35"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="38" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58" s="37" t="s">
-        <v>1735</v>
-      </c>
-      <c r="C58" s="35"/>
-      <c r="D58" s="35"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="38" t="s">
-        <v>1759</v>
-      </c>
-      <c r="B59" s="37" t="s">
-        <v>1736</v>
-      </c>
-      <c r="C59" s="35"/>
-      <c r="D59" s="35"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="38" t="s">
-        <v>1759</v>
-      </c>
-      <c r="B60" s="37" t="s">
-        <v>1737</v>
-      </c>
-      <c r="C60" s="35"/>
-      <c r="D60" s="35"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="38" t="s">
-        <v>1759</v>
-      </c>
-      <c r="B61" s="37" t="s">
-        <v>1738</v>
-      </c>
-      <c r="C61" s="35"/>
-      <c r="D61" s="35"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="38" t="s">
-        <v>1759</v>
-      </c>
-      <c r="B62" s="37" t="s">
-        <v>1739</v>
-      </c>
-      <c r="C62" s="35"/>
-      <c r="D62" s="35"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B63" s="37" t="s">
-        <v>1740</v>
-      </c>
-      <c r="C63" s="35"/>
-      <c r="D63" s="35"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B64" s="37" t="s">
-        <v>1741</v>
-      </c>
-      <c r="C64" s="35"/>
-      <c r="D64" s="35"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B65" s="37" t="s">
-        <v>1742</v>
-      </c>
-      <c r="C65" s="35"/>
-      <c r="D65" s="35"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B66" s="37" t="s">
-        <v>1743</v>
-      </c>
-      <c r="C66" s="35"/>
-      <c r="D66" s="35"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B67" s="37" t="s">
-        <v>1744</v>
-      </c>
-      <c r="C67" s="35"/>
-      <c r="D67" s="35"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B68" s="37" t="s">
-        <v>1745</v>
-      </c>
-      <c r="C68" s="35"/>
-      <c r="D68" s="35"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B69" s="37" t="s">
-        <v>1746</v>
-      </c>
-      <c r="C69" s="35"/>
-      <c r="D69" s="35"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B70" s="37" t="s">
-        <v>1747</v>
-      </c>
-      <c r="C70" s="35"/>
-      <c r="D70" s="35"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B71" s="37" t="s">
-        <v>1748</v>
-      </c>
-      <c r="C71" s="35"/>
-      <c r="D71" s="35"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B72" s="37" t="s">
-        <v>1749</v>
-      </c>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B73" s="37" t="s">
-        <v>1750</v>
-      </c>
-      <c r="C73" s="35"/>
-      <c r="D73" s="35"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B74" s="37" t="s">
-        <v>1751</v>
-      </c>
-      <c r="C74" s="35"/>
-      <c r="D74" s="35"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B75" s="37" t="s">
-        <v>1752</v>
-      </c>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B76" s="37" t="s">
-        <v>1753</v>
-      </c>
-      <c r="C76" s="35"/>
-      <c r="D76" s="35"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="39" t="s">
-        <v>1760</v>
-      </c>
-      <c r="B77" s="37" t="s">
-        <v>1754</v>
-      </c>
-      <c r="C77" s="35"/>
-      <c r="D77" s="35"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -27208,7 +26106,7 @@
   <dimension ref="A2:D391"/>
   <sheetViews>
     <sheetView topLeftCell="A349" workbookViewId="0">
-      <selection activeCell="D362" sqref="D362"/>
+      <selection activeCell="A2" sqref="A2:D367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add New test secnario09
</commit_message>
<xml_diff>
--- a/INOW Automation Data Sheet.xlsx
+++ b/INOW Automation Data Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InsuranceNowAutomation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\InsuranceNowAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27AEE311-CAFF-4114-9353-2E5CAD12CA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BA0F24D-6571-4CB2-8AD8-4A247EABDEDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="16" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="11" activeTab="17" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NewBussines" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,8 @@
     <sheet name="Batch Job" sheetId="31" r:id="rId15"/>
     <sheet name="TS_01" sheetId="25" r:id="rId16"/>
     <sheet name="TS_02" sheetId="28" r:id="rId17"/>
-    <sheet name="TS_03" sheetId="29" r:id="rId18"/>
+    <sheet name="TS_05" sheetId="32" r:id="rId18"/>
+    <sheet name="TS_03" sheetId="29" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6404" uniqueCount="1688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6423" uniqueCount="1694">
   <si>
     <t>NewBussines</t>
   </si>
@@ -5117,6 +5118,24 @@
   </si>
   <si>
     <t>endorsementNonDriver2Gender</t>
+  </si>
+  <si>
+    <t>hoa</t>
+  </si>
+  <si>
+    <t>renewalPolicyNumber</t>
+  </si>
+  <si>
+    <t>Renewal Start Done</t>
+  </si>
+  <si>
+    <t>renewalStartTransaction</t>
+  </si>
+  <si>
+    <t>renewalStartDescription</t>
+  </si>
+  <si>
+    <t>PA0000017-01</t>
   </si>
 </sst>
 </file>
@@ -9625,7 +9644,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5456E97C-0A17-42B4-A214-4BA726B8ADBA}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="BO1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -14269,7 +14288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE3BCC8-1641-433F-8FC0-0BC9EA113D75}">
   <dimension ref="D1:G736"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A525" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A522" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F539" sqref="F539"/>
     </sheetView>
   </sheetViews>
@@ -21775,12 +21794,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D174:D277"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D3:D49"/>
-    <mergeCell ref="D50:D59"/>
-    <mergeCell ref="D60:D157"/>
-    <mergeCell ref="D158:D173"/>
     <mergeCell ref="D524:D539"/>
     <mergeCell ref="D540:D643"/>
     <mergeCell ref="D644:D697"/>
@@ -21791,6 +21804,12 @@
     <mergeCell ref="D373:D415"/>
     <mergeCell ref="D416:D425"/>
     <mergeCell ref="D426:D523"/>
+    <mergeCell ref="D174:D277"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D3:D49"/>
+    <mergeCell ref="D50:D59"/>
+    <mergeCell ref="D60:D157"/>
+    <mergeCell ref="D158:D173"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G44" r:id="rId1" xr:uid="{249BC4C0-3423-4E91-A0D7-112396468B55}"/>
@@ -21801,10 +21820,139 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C769D613-2896-45AA-B7E3-BA8DD5AD2AD8}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>1688</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13"/>
+      <c r="B3" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1689</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1691</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1692</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC48D60B-A2DA-4B33-8870-4BC720D13BF5}">
   <dimension ref="A1:D416"/>
   <sheetViews>
-    <sheetView topLeftCell="A380" workbookViewId="0">
+    <sheetView topLeftCell="A395" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -26106,18 +26254,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A174:A277"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A49"/>
+    <mergeCell ref="A50:A59"/>
+    <mergeCell ref="A60:A157"/>
+    <mergeCell ref="A158:A173"/>
     <mergeCell ref="A371:D371"/>
     <mergeCell ref="A381:D381"/>
     <mergeCell ref="A391:D391"/>
     <mergeCell ref="A403:D403"/>
     <mergeCell ref="A278:A331"/>
     <mergeCell ref="A332:A353"/>
-    <mergeCell ref="A174:A277"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A49"/>
-    <mergeCell ref="A50:A59"/>
-    <mergeCell ref="A60:A157"/>
-    <mergeCell ref="A158:A173"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D44" r:id="rId1" xr:uid="{DE8D0F4F-6169-48C2-82D8-7C8293E1696B}"/>
@@ -34293,7 +34441,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C6"/>
+      <selection sqref="A1:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Endorsement eff date updated & endorsement policy number change
</commit_message>
<xml_diff>
--- a/INOW Automation Data Sheet.xlsx
+++ b/INOW Automation Data Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InsuranceNowAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF3E5255-B20C-4B74-8E89-D8173689457B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4641E07E-EE0D-4201-A193-4FEC6AE93F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="11" activeTab="16" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="12" activeTab="16" xr2:uid="{1D5F82B1-D089-4CF0-BE2B-D18622951DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="NewBussines" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,8 @@
     <sheet name="Batch Job" sheetId="31" r:id="rId15"/>
     <sheet name="TS_01" sheetId="25" r:id="rId16"/>
     <sheet name="TS_02" sheetId="28" r:id="rId17"/>
-    <sheet name="TS_03" sheetId="29" r:id="rId18"/>
+    <sheet name="NBPolicyNumber" sheetId="32" r:id="rId18"/>
+    <sheet name="TS_03" sheetId="29" r:id="rId19"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6405" uniqueCount="1691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6407" uniqueCount="1693">
   <si>
     <t>NewBussines</t>
   </si>
@@ -4831,9 +4832,6 @@
     <t>10/01/2023</t>
   </si>
   <si>
-    <t>10/02/2023</t>
-  </si>
-  <si>
     <t>Post</t>
   </si>
   <si>
@@ -5126,6 +5124,15 @@
   </si>
   <si>
     <t>endorsementVehicle1TowingAndLabor</t>
+  </si>
+  <si>
+    <t>NewBusiness03PolicyNumber</t>
+  </si>
+  <si>
+    <t>NewBusiness04PolicyNumber</t>
+  </si>
+  <si>
+    <t>10/11/2023</t>
   </si>
 </sst>
 </file>
@@ -9869,7 +9876,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -9895,7 +9902,7 @@
         <v>355</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -9905,7 +9912,7 @@
         <v>355</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -9915,7 +9922,7 @@
         <v>355</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -9925,7 +9932,7 @@
         <v>355</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -9935,7 +9942,7 @@
         <v>355</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -9945,7 +9952,7 @@
         <v>355</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -9955,7 +9962,7 @@
         <v>355</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -9965,7 +9972,7 @@
         <v>355</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -9975,7 +9982,7 @@
         <v>355</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -9985,7 +9992,7 @@
         <v>355</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -10045,7 +10052,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -10071,7 +10078,7 @@
         <v>355</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -10081,7 +10088,7 @@
         <v>355</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -10091,7 +10098,7 @@
         <v>355</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -10101,7 +10108,7 @@
         <v>355</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -10111,7 +10118,7 @@
         <v>355</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -10121,7 +10128,7 @@
         <v>355</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -10131,7 +10138,7 @@
         <v>355</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -10141,7 +10148,7 @@
         <v>355</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -10151,7 +10158,7 @@
         <v>355</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -10161,7 +10168,7 @@
         <v>355</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -10171,7 +10178,7 @@
         <v>355</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -10181,7 +10188,7 @@
         <v>355</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -10331,7 +10338,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>25</v>
@@ -10970,7 +10977,7 @@
         <v>1565</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -14003,7 +14010,7 @@
     </row>
     <row r="371" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A371" s="30" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="B371" s="30"/>
       <c r="C371" s="30"/>
@@ -14015,7 +14022,7 @@
         <v>7</v>
       </c>
       <c r="C372" s="1" t="s">
-        <v>1642</v>
+        <v>1641</v>
       </c>
       <c r="D372" s="1" t="s">
         <v>1542</v>
@@ -14027,10 +14034,10 @@
         <v>7</v>
       </c>
       <c r="C373" s="1" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="D373" s="1" t="s">
-        <v>1659</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="374" spans="1:4" x14ac:dyDescent="0.25">
@@ -14039,7 +14046,7 @@
         <v>7</v>
       </c>
       <c r="C374" s="1" t="s">
-        <v>1643</v>
+        <v>1642</v>
       </c>
       <c r="D374" s="1"/>
     </row>
@@ -14049,10 +14056,10 @@
         <v>7</v>
       </c>
       <c r="C375" s="2" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>1660</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
@@ -14061,7 +14068,7 @@
         <v>7</v>
       </c>
       <c r="C376" s="2" t="s">
-        <v>1644</v>
+        <v>1643</v>
       </c>
       <c r="D376" s="1"/>
     </row>
@@ -14071,43 +14078,43 @@
         <v>7</v>
       </c>
       <c r="C377" s="2" t="s">
-        <v>1645</v>
+        <v>1644</v>
       </c>
       <c r="D377" s="17" t="s">
-        <v>1661</v>
+        <v>1660</v>
       </c>
     </row>
     <row r="378" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A378" s="1"/>
       <c r="B378" s="2" t="s">
+        <v>1661</v>
+      </c>
+      <c r="C378" s="2" t="s">
         <v>1662</v>
       </c>
-      <c r="C378" s="2" t="s">
-        <v>1663</v>
-      </c>
       <c r="D378" s="1" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="379" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A379" s="1"/>
       <c r="B379" s="2" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="C379" s="2" t="s">
-        <v>1664</v>
+        <v>1663</v>
       </c>
       <c r="D379" s="1" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="380" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A380" s="1"/>
       <c r="B380" s="2" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="C380" s="1" t="s">
-        <v>1665</v>
+        <v>1664</v>
       </c>
       <c r="D380" s="1" t="s">
         <v>1536</v>
@@ -14116,13 +14123,13 @@
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A381" s="1"/>
       <c r="B381" s="2" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="C381" s="1" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="D381" s="17" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="382" spans="1:4" x14ac:dyDescent="0.25">
@@ -14131,10 +14138,10 @@
         <v>9</v>
       </c>
       <c r="C382" s="1" t="s">
-        <v>1646</v>
+        <v>1645</v>
       </c>
       <c r="D382" s="1" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="383" spans="1:4" x14ac:dyDescent="0.25">
@@ -14143,10 +14150,10 @@
         <v>9</v>
       </c>
       <c r="C383" s="1" t="s">
+        <v>1670</v>
+      </c>
+      <c r="D383" s="17" t="s">
         <v>1671</v>
-      </c>
-      <c r="D383" s="17" t="s">
-        <v>1672</v>
       </c>
     </row>
     <row r="384" spans="1:4" x14ac:dyDescent="0.25">
@@ -14155,7 +14162,7 @@
         <v>9</v>
       </c>
       <c r="C384" s="5" t="s">
-        <v>1647</v>
+        <v>1646</v>
       </c>
       <c r="D384" s="1" t="s">
         <v>1548</v>
@@ -14167,7 +14174,7 @@
         <v>9</v>
       </c>
       <c r="C385" s="1" t="s">
-        <v>1648</v>
+        <v>1647</v>
       </c>
       <c r="D385" s="1" t="s">
         <v>1543</v>
@@ -14179,7 +14186,7 @@
         <v>9</v>
       </c>
       <c r="C386" s="1" t="s">
-        <v>1649</v>
+        <v>1648</v>
       </c>
       <c r="D386" s="1" t="s">
         <v>1544</v>
@@ -14187,7 +14194,7 @@
     </row>
     <row r="387" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A387" s="30" t="s">
-        <v>1650</v>
+        <v>1649</v>
       </c>
       <c r="B387" s="30"/>
       <c r="C387" s="30"/>
@@ -14196,46 +14203,46 @@
     <row r="388" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A388" s="1"/>
       <c r="B388" s="1" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="C388" s="13" t="s">
-        <v>1651</v>
+        <v>1650</v>
       </c>
       <c r="D388" s="1" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
     </row>
     <row r="389" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A389" s="1"/>
       <c r="B389" s="1" t="s">
+        <v>1655</v>
+      </c>
+      <c r="C389" s="13" t="s">
+        <v>1651</v>
+      </c>
+      <c r="D389" s="17" t="s">
         <v>1656</v>
-      </c>
-      <c r="C389" s="13" t="s">
-        <v>1652</v>
-      </c>
-      <c r="D389" s="17" t="s">
-        <v>1657</v>
       </c>
     </row>
     <row r="390" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A390" s="1"/>
       <c r="B390" s="1" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="C390" s="13" t="s">
-        <v>1653</v>
+        <v>1652</v>
       </c>
       <c r="D390" s="17" t="s">
-        <v>1658</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" s="1"/>
       <c r="B391" s="1" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="C391" s="13" t="s">
-        <v>1654</v>
+        <v>1653</v>
       </c>
       <c r="D391" s="1" t="s">
         <v>1536</v>
@@ -14244,10 +14251,10 @@
     <row r="392" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A392" s="1"/>
       <c r="B392" s="1" t="s">
-        <v>1656</v>
+        <v>1655</v>
       </c>
       <c r="C392" s="13" t="s">
-        <v>1655</v>
+        <v>1654</v>
       </c>
       <c r="D392" s="1" t="s">
         <v>1537</v>
@@ -14278,8 +14285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FE3BCC8-1641-433F-8FC0-0BC9EA113D75}">
   <dimension ref="D1:G736"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A718" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F722" sqref="F722"/>
+    <sheetView tabSelected="1" topLeftCell="A362" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G373" sqref="G373"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14379,7 +14386,7 @@
         <v>1575</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>1606</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.25">
@@ -18105,7 +18112,7 @@
         <v>37</v>
       </c>
       <c r="G373" s="16" t="s">
-        <v>1592</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="374" spans="4:7" x14ac:dyDescent="0.25">
@@ -19617,7 +19624,7 @@
         <v>159</v>
       </c>
       <c r="G524" s="1" t="s">
-        <v>1593</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="525" spans="4:7" x14ac:dyDescent="0.25">
@@ -19636,10 +19643,10 @@
         <v>15</v>
       </c>
       <c r="F526" s="1" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="G526" s="1" t="s">
-        <v>1594</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="527" spans="4:7" x14ac:dyDescent="0.25">
@@ -19648,10 +19655,10 @@
         <v>15</v>
       </c>
       <c r="F527" s="1" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="G527" s="1" t="s">
-        <v>1595</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="528" spans="4:7" x14ac:dyDescent="0.25">
@@ -19660,10 +19667,10 @@
         <v>15</v>
       </c>
       <c r="F528" s="1" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="G528" s="1" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="529" spans="4:7" x14ac:dyDescent="0.25">
@@ -19672,7 +19679,7 @@
         <v>15</v>
       </c>
       <c r="F529" s="1" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="G529" s="1" t="s">
         <v>1558</v>
@@ -19687,7 +19694,7 @@
         <v>165</v>
       </c>
       <c r="G530" s="17" t="s">
-        <v>1596</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="531" spans="4:7" x14ac:dyDescent="0.25">
@@ -19699,7 +19706,7 @@
         <v>166</v>
       </c>
       <c r="G531" s="1" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="532" spans="4:7" x14ac:dyDescent="0.25">
@@ -19711,7 +19718,7 @@
         <v>167</v>
       </c>
       <c r="G532" s="1" t="s">
-        <v>1598</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="533" spans="4:7" x14ac:dyDescent="0.25">
@@ -19720,7 +19727,7 @@
         <v>15</v>
       </c>
       <c r="F533" s="1" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="G533" s="1"/>
     </row>
@@ -19730,10 +19737,10 @@
         <v>15</v>
       </c>
       <c r="F534" s="1" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="G534" s="1" t="s">
-        <v>1599</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="535" spans="4:7" x14ac:dyDescent="0.25">
@@ -19742,10 +19749,10 @@
         <v>15</v>
       </c>
       <c r="F535" s="1" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="G535" s="1" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="536" spans="4:7" x14ac:dyDescent="0.25">
@@ -19754,10 +19761,10 @@
         <v>15</v>
       </c>
       <c r="F536" s="1" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="G536" s="1" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="537" spans="4:7" x14ac:dyDescent="0.25">
@@ -19766,10 +19773,10 @@
         <v>15</v>
       </c>
       <c r="F537" s="1" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="G537" s="1" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="538" spans="4:7" x14ac:dyDescent="0.25">
@@ -19781,7 +19788,7 @@
         <v>173</v>
       </c>
       <c r="G538" s="17" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="539" spans="4:7" x14ac:dyDescent="0.25">
@@ -19793,7 +19800,7 @@
         <v>174</v>
       </c>
       <c r="G539" s="1" t="s">
-        <v>1597</v>
+        <v>1596</v>
       </c>
     </row>
     <row r="540" spans="4:7" x14ac:dyDescent="0.25">
@@ -19807,7 +19814,7 @@
         <v>175</v>
       </c>
       <c r="G540" s="1" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="541" spans="4:7" x14ac:dyDescent="0.25">
@@ -19918,7 +19925,7 @@
         <v>16</v>
       </c>
       <c r="F551" s="1" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="G551" s="1" t="s">
         <v>1569</v>
@@ -20016,7 +20023,7 @@
         <v>16</v>
       </c>
       <c r="F560" s="1" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="G560" s="1" t="s">
         <v>1571</v>
@@ -21399,7 +21406,7 @@
         <v>260</v>
       </c>
       <c r="G698" s="1" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="699" spans="4:7" x14ac:dyDescent="0.25">
@@ -21411,7 +21418,7 @@
         <v>261</v>
       </c>
       <c r="G699" s="1" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="700" spans="4:7" x14ac:dyDescent="0.25">
@@ -21786,12 +21793,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D174:D277"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="D3:D49"/>
-    <mergeCell ref="D50:D59"/>
-    <mergeCell ref="D60:D157"/>
-    <mergeCell ref="D158:D173"/>
     <mergeCell ref="D524:D539"/>
     <mergeCell ref="D540:D643"/>
     <mergeCell ref="D644:D697"/>
@@ -21802,6 +21803,12 @@
     <mergeCell ref="D373:D415"/>
     <mergeCell ref="D416:D425"/>
     <mergeCell ref="D426:D523"/>
+    <mergeCell ref="D174:D277"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="D3:D49"/>
+    <mergeCell ref="D50:D59"/>
+    <mergeCell ref="D60:D157"/>
+    <mergeCell ref="D158:D173"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G44" r:id="rId1" xr:uid="{249BC4C0-3423-4E91-A0D7-112396468B55}"/>
@@ -21812,6 +21819,34 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{812DB0A4-DE2B-48B4-ADFF-E7310E8380F2}">
+  <dimension ref="B3:B4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1690</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>1691</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC48D60B-A2DA-4B33-8870-4BC720D13BF5}">
   <dimension ref="A1:D416"/>
   <sheetViews>
@@ -21829,7 +21864,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>1641</v>
+        <v>1640</v>
       </c>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
@@ -25660,7 +25695,7 @@
         <v>363</v>
       </c>
       <c r="D374" s="17" t="s">
-        <v>1631</v>
+        <v>1630</v>
       </c>
     </row>
     <row r="375" spans="1:4" x14ac:dyDescent="0.25">
@@ -25672,7 +25707,7 @@
         <v>364</v>
       </c>
       <c r="D375" s="1" t="s">
-        <v>1632</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="376" spans="1:4" x14ac:dyDescent="0.25">
@@ -25724,7 +25759,7 @@
         <v>369</v>
       </c>
       <c r="D380" s="1" t="s">
-        <v>1633</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="381" spans="1:4" x14ac:dyDescent="0.25">
@@ -25831,7 +25866,7 @@
     </row>
     <row r="391" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A391" s="29" t="s">
-        <v>1607</v>
+        <v>1606</v>
       </c>
       <c r="B391" s="29"/>
       <c r="C391" s="29"/>
@@ -25857,10 +25892,10 @@
         <v>355</v>
       </c>
       <c r="C393" s="1" t="s">
-        <v>1608</v>
+        <v>1607</v>
       </c>
       <c r="D393" s="20" t="s">
-        <v>1634</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="394" spans="1:4" x14ac:dyDescent="0.25">
@@ -25869,7 +25904,7 @@
         <v>355</v>
       </c>
       <c r="C394" s="1" t="s">
-        <v>1609</v>
+        <v>1608</v>
       </c>
       <c r="D394" s="1"/>
     </row>
@@ -25879,10 +25914,10 @@
         <v>355</v>
       </c>
       <c r="C395" s="1" t="s">
-        <v>1610</v>
+        <v>1609</v>
       </c>
       <c r="D395" s="21" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="396" spans="1:4" x14ac:dyDescent="0.25">
@@ -25891,10 +25926,10 @@
         <v>355</v>
       </c>
       <c r="C396" s="1" t="s">
-        <v>1611</v>
+        <v>1610</v>
       </c>
       <c r="D396" s="21" t="s">
-        <v>1639</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="397" spans="1:4" x14ac:dyDescent="0.25">
@@ -25903,7 +25938,7 @@
         <v>355</v>
       </c>
       <c r="C397" s="1" t="s">
-        <v>1612</v>
+        <v>1611</v>
       </c>
       <c r="D397" s="1" t="s">
         <v>25</v>
@@ -25915,10 +25950,10 @@
         <v>355</v>
       </c>
       <c r="C398" s="1" t="s">
-        <v>1613</v>
+        <v>1612</v>
       </c>
       <c r="D398" s="1" t="s">
-        <v>1635</v>
+        <v>1634</v>
       </c>
     </row>
     <row r="399" spans="1:4" x14ac:dyDescent="0.25">
@@ -25927,10 +25962,10 @@
         <v>355</v>
       </c>
       <c r="C399" s="1" t="s">
-        <v>1614</v>
+        <v>1613</v>
       </c>
       <c r="D399" s="1" t="s">
-        <v>1636</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="400" spans="1:4" x14ac:dyDescent="0.25">
@@ -25939,10 +25974,10 @@
         <v>355</v>
       </c>
       <c r="C400" s="1" t="s">
-        <v>1615</v>
+        <v>1614</v>
       </c>
       <c r="D400" s="17" t="s">
-        <v>1637</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="401" spans="1:4" x14ac:dyDescent="0.25">
@@ -25951,10 +25986,10 @@
         <v>355</v>
       </c>
       <c r="C401" s="1" t="s">
-        <v>1616</v>
+        <v>1615</v>
       </c>
       <c r="D401" s="17" t="s">
-        <v>1638</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="402" spans="1:4" x14ac:dyDescent="0.25">
@@ -25963,7 +25998,7 @@
         <v>355</v>
       </c>
       <c r="C402" s="1" t="s">
-        <v>1617</v>
+        <v>1616</v>
       </c>
       <c r="D402" s="1" t="s">
         <v>1587</v>
@@ -25971,7 +26006,7 @@
     </row>
     <row r="403" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A403" s="29" t="s">
-        <v>1618</v>
+        <v>1617</v>
       </c>
       <c r="B403" s="29"/>
       <c r="C403" s="29"/>
@@ -25997,10 +26032,10 @@
         <v>355</v>
       </c>
       <c r="C405" s="1" t="s">
-        <v>1619</v>
+        <v>1618</v>
       </c>
       <c r="D405" s="17" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="406" spans="1:4" x14ac:dyDescent="0.25">
@@ -26009,10 +26044,10 @@
         <v>355</v>
       </c>
       <c r="C406" s="1" t="s">
-        <v>1620</v>
+        <v>1619</v>
       </c>
       <c r="D406" s="17" t="s">
-        <v>1640</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="407" spans="1:4" x14ac:dyDescent="0.25">
@@ -26021,7 +26056,7 @@
         <v>355</v>
       </c>
       <c r="C407" s="1" t="s">
-        <v>1621</v>
+        <v>1620</v>
       </c>
       <c r="D407" s="1"/>
     </row>
@@ -26031,7 +26066,7 @@
         <v>355</v>
       </c>
       <c r="C408" s="1" t="s">
-        <v>1622</v>
+        <v>1621</v>
       </c>
       <c r="D408" s="1"/>
     </row>
@@ -26041,7 +26076,7 @@
         <v>355</v>
       </c>
       <c r="C409" s="2" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
       <c r="D409" s="1"/>
     </row>
@@ -26051,7 +26086,7 @@
         <v>355</v>
       </c>
       <c r="C410" s="1" t="s">
-        <v>1624</v>
+        <v>1623</v>
       </c>
       <c r="D410" s="1"/>
     </row>
@@ -26061,7 +26096,7 @@
         <v>355</v>
       </c>
       <c r="C411" s="1" t="s">
-        <v>1625</v>
+        <v>1624</v>
       </c>
       <c r="D411" s="1"/>
     </row>
@@ -26071,7 +26106,7 @@
         <v>355</v>
       </c>
       <c r="C412" s="1" t="s">
-        <v>1626</v>
+        <v>1625</v>
       </c>
       <c r="D412" s="1"/>
     </row>
@@ -26081,7 +26116,7 @@
         <v>355</v>
       </c>
       <c r="C413" s="1" t="s">
-        <v>1627</v>
+        <v>1626</v>
       </c>
       <c r="D413" s="1"/>
     </row>
@@ -26091,7 +26126,7 @@
         <v>355</v>
       </c>
       <c r="C414" s="1" t="s">
-        <v>1628</v>
+        <v>1627</v>
       </c>
       <c r="D414" s="1"/>
     </row>
@@ -26101,7 +26136,7 @@
         <v>355</v>
       </c>
       <c r="C415" s="2" t="s">
-        <v>1629</v>
+        <v>1628</v>
       </c>
       <c r="D415" s="1"/>
     </row>
@@ -26111,24 +26146,24 @@
         <v>355</v>
       </c>
       <c r="C416" s="1" t="s">
-        <v>1630</v>
+        <v>1629</v>
       </c>
       <c r="D416" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A174:A277"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A3:A49"/>
+    <mergeCell ref="A50:A59"/>
+    <mergeCell ref="A60:A157"/>
+    <mergeCell ref="A158:A173"/>
     <mergeCell ref="A371:D371"/>
     <mergeCell ref="A381:D381"/>
     <mergeCell ref="A391:D391"/>
     <mergeCell ref="A403:D403"/>
     <mergeCell ref="A278:A331"/>
     <mergeCell ref="A332:A353"/>
-    <mergeCell ref="A174:A277"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:A49"/>
-    <mergeCell ref="A50:A59"/>
-    <mergeCell ref="A60:A157"/>
-    <mergeCell ref="A158:A173"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D44" r:id="rId1" xr:uid="{DE8D0F4F-6169-48C2-82D8-7C8293E1696B}"/>

</xml_diff>